<commit_message>
Made the font center better
</commit_message>
<xml_diff>
--- a/Resources/Bracket.xlsx
+++ b/Resources/Bracket.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pants\IdeaProjects\Mam\Resources\"/>
     </mc:Choice>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6341" uniqueCount="81">
   <si>
     <t>Type in the two Wildcard animals below</t>
   </si>
@@ -185,12 +185,109 @@
   </si>
   <si>
     <t>Itjaritjari</t>
+  </si>
+  <si>
+    <t>Striped dolphin</t>
+  </si>
+  <si>
+    <t>New Caledonian Crow</t>
+  </si>
+  <si>
+    <t>Kudu</t>
+  </si>
+  <si>
+    <t>Silver Pika</t>
+  </si>
+  <si>
+    <t>Peacock Wrasse</t>
+  </si>
+  <si>
+    <t>Mara</t>
+  </si>
+  <si>
+    <t>Bat-Eared Fox</t>
+  </si>
+  <si>
+    <t>Colo Colo Opossum</t>
+  </si>
+  <si>
+    <t>Giant Water Bug</t>
+  </si>
+  <si>
+    <t>Bulldog Bat</t>
+  </si>
+  <si>
+    <t>Shrew Mole</t>
+  </si>
+  <si>
+    <t>Puffer Fish</t>
+  </si>
+  <si>
+    <t>Trapdoor Spider</t>
+  </si>
+  <si>
+    <t>Highland Streaked Tenrec</t>
+  </si>
+  <si>
+    <t>Rufous Hornero</t>
+  </si>
+  <si>
+    <t>Silky Anteater</t>
+  </si>
+  <si>
+    <t>Pygmy Jerboa</t>
+  </si>
+  <si>
+    <t>Striped Polecat</t>
+  </si>
+  <si>
+    <t>Bee</t>
+  </si>
+  <si>
+    <t>Grasshopper Mouse</t>
+  </si>
+  <si>
+    <t>Caspian Terns</t>
+  </si>
+  <si>
+    <t>Dyak Fruit Bat</t>
+  </si>
+  <si>
+    <t>Striped Possum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Three-Spined stickleback </t>
+  </si>
+  <si>
+    <t>Numbat</t>
+  </si>
+  <si>
+    <t>Four-Striped Grass Mouse</t>
+  </si>
+  <si>
+    <t>Lined Seahorse</t>
+  </si>
+  <si>
+    <t>Dung Beetle</t>
+  </si>
+  <si>
+    <t>Fire-footed Rope Squirrel</t>
+  </si>
+  <si>
+    <t>Tent-making Bat</t>
+  </si>
+  <si>
+    <t>Spongilla Fly</t>
+  </si>
+  <si>
+    <t>Darwin's Frogs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -892,10 +989,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.140625" customWidth="1"/>
-    <col min="2" max="2" width="41.28515625" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1"/>
-    <col min="4" max="4" width="25" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="36.140625"/>
+    <col min="2" max="2" customWidth="true" width="41.28515625"/>
+    <col min="3" max="3" customWidth="true" width="18.42578125"/>
+    <col min="4" max="4" customWidth="true" width="25.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1782,774 +1879,774 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" customWidth="1"/>
-    <col min="15" max="15" width="23.42578125" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="14.7109375"/>
+    <col min="3" max="3" customWidth="true" width="25.42578125"/>
+    <col min="15" max="15" customWidth="true" width="23.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1">
+      <c r="A1" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="str">
+      <c r="C1" t="str" s="0">
         <f>Helper!D2</f>
         <v>Okapi</v>
       </c>
-      <c r="O1" t="str">
+      <c r="O1" t="str" s="0">
         <f>Helper!D35</f>
         <v>Golden Eagle</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="0">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="D2" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="N2" t="s" s="0">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="0">
         <v>3</v>
       </c>
-      <c r="C3" t="str">
+      <c r="C3" t="str" s="0">
         <f>Helper!D17</f>
         <v>Four-Striped Grass Mouse</v>
       </c>
-      <c r="O3" t="str">
+      <c r="O3" t="str" s="0">
         <f>Helper!D50</f>
         <v>Spongilla Fly</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>4</v>
-      </c>
-      <c r="E4" t="s">
-        <v>4</v>
-      </c>
-      <c r="M4" t="s">
+      <c r="A4" s="0">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="M4" t="s" s="0">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="0">
         <v>5</v>
       </c>
-      <c r="C5" t="str">
+      <c r="C5" t="str" s="0">
         <f>Helper!D9</f>
         <v>Striped Polecat</v>
       </c>
-      <c r="O5" t="str">
+      <c r="O5" t="str" s="0">
         <f>Helper!D42</f>
         <v>Veined Octopus</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="0">
         <v>6</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="N6" t="s">
+      <c r="N6" t="s" s="0">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="0">
         <v>7</v>
       </c>
-      <c r="C7" t="str">
+      <c r="C7" t="str" s="0">
         <f>Helper!D10</f>
         <v>Giant striped mongoose</v>
       </c>
-      <c r="O7" t="str">
+      <c r="O7" t="str" s="0">
         <f>Helper!D43</f>
         <v>Puffer Fish</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="0">
         <v>8</v>
       </c>
-      <c r="F8" t="s">
-        <v>4</v>
-      </c>
-      <c r="L8" t="s">
+      <c r="F8" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="L8" t="s" s="0">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="0">
         <v>9</v>
       </c>
-      <c r="C9" t="str">
+      <c r="C9" t="str" s="0">
         <f>Helper!D6</f>
         <v>Side-striped jackal</v>
       </c>
-      <c r="O9" t="str">
+      <c r="O9" t="str" s="0">
         <f>Helper!D39</f>
         <v>Palaeocastor</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" s="0">
         <v>10</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="N10" t="s">
+      <c r="N10" t="s" s="0">
         <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="0">
         <v>11</v>
       </c>
-      <c r="C11" t="str">
+      <c r="C11" t="str" s="0">
         <f>Helper!D13</f>
         <v>Striped Possum</v>
       </c>
-      <c r="O11" t="str">
+      <c r="O11" t="str" s="0">
         <f>Helper!D46</f>
         <v>Trapdoor Spider</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="0">
         <v>12</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="M12" t="s">
+      <c r="M12" t="s" s="0">
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" s="0">
         <v>13</v>
       </c>
-      <c r="C13" t="str">
+      <c r="C13" t="str" s="0">
         <f>Helper!D5</f>
         <v>Striped dolphin</v>
       </c>
-      <c r="O13" t="str">
+      <c r="O13" t="str" s="0">
         <f>Helper!D38</f>
         <v>Lungfish</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="A14" s="0">
         <v>14</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="N14" t="s">
+      <c r="N14" t="s" s="0">
         <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="A15" s="0">
         <v>15</v>
       </c>
-      <c r="C15" t="str">
+      <c r="C15" t="str" s="0">
         <f>Helper!D14</f>
         <v>Chequered elephant shrew</v>
       </c>
-      <c r="O15" t="str">
+      <c r="O15" t="str" s="0">
         <f>Helper!D47</f>
         <v>Tent-making Bat</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="A16" s="0">
         <v>16</v>
       </c>
-      <c r="G16" t="s">
-        <v>4</v>
-      </c>
-      <c r="K16" t="s">
+      <c r="G16" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="K16" t="s" s="0">
         <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="A17" s="0">
         <v>17</v>
       </c>
-      <c r="C17" t="str">
+      <c r="C17" t="str" s="0">
         <f>Helper!D7</f>
         <v>Wildcat</v>
       </c>
-      <c r="O17" t="str">
+      <c r="O17" t="str" s="0">
         <f>Helper!D40</f>
         <v>Goanna</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="A18" s="0">
         <v>18</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="N18" t="s">
+      <c r="N18" t="s" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="A19" s="0">
         <v>19</v>
       </c>
-      <c r="C19" t="str">
+      <c r="C19" t="str" s="0">
         <f>Helper!D12</f>
         <v>Highland Streaked Tenrec</v>
       </c>
-      <c r="O19" t="str">
+      <c r="O19" t="str" s="0">
         <f>Helper!D45</f>
         <v>Rufous Hornero</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="A20" s="0">
         <v>20</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="M20" t="s">
+      <c r="M20" t="s" s="0">
         <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="A21" s="0">
         <v>21</v>
       </c>
-      <c r="C21" t="str">
+      <c r="C21" t="str" s="0">
         <f>Helper!D4</f>
         <v>Striped hyena</v>
       </c>
-      <c r="O21" t="str">
+      <c r="O21" t="str" s="0">
         <f>Helper!D37</f>
         <v>Homo habilis</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="A22" s="0">
         <v>22</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="N22" t="s">
+      <c r="N22" t="s" s="0">
         <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="A23" s="0">
         <v>23</v>
       </c>
-      <c r="C23" t="str">
+      <c r="C23" t="str" s="0">
         <f>Helper!D15</f>
         <v>Fire-footed Rope Squirrel</v>
       </c>
-      <c r="O23" t="str">
+      <c r="O23" t="str" s="0">
         <f>Helper!D48</f>
         <v>Bee</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24">
+      <c r="A24" s="0">
         <v>24</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="L24" t="s">
+      <c r="L24" t="s" s="0">
         <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25">
+      <c r="A25" s="0">
         <v>25</v>
       </c>
-      <c r="C25" t="str">
+      <c r="C25" t="str" s="0">
         <f>Helper!D8</f>
         <v>Striped Rabbit</v>
       </c>
-      <c r="O25" t="str">
+      <c r="O25" t="str" s="0">
         <f>Helper!D41</f>
         <v>Montezuma Oropendola</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26">
+      <c r="A26" s="0">
         <v>26</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="N26" t="s">
+      <c r="N26" t="s" s="0">
         <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27">
+      <c r="A27" s="0">
         <v>27</v>
       </c>
-      <c r="C27" t="str">
+      <c r="C27" t="str" s="0">
         <f>Helper!D11</f>
         <v>Numbat</v>
       </c>
-      <c r="O27" t="str">
+      <c r="O27" t="str" s="0">
         <f>Helper!D44</f>
         <v>New Caledonian Crow</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28">
+      <c r="A28" s="0">
         <v>28</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="M28" t="s">
+      <c r="M28" t="s" s="0">
         <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29">
+      <c r="A29" s="0">
         <v>29</v>
       </c>
-      <c r="C29" t="str">
+      <c r="C29" t="str" s="0">
         <f>Helper!D3</f>
         <v>Kudu</v>
       </c>
-      <c r="O29" t="str">
+      <c r="O29" t="str" s="0">
         <f>Helper!D36</f>
         <v>Cathedral Termite</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30">
+      <c r="A30" s="0">
         <v>30</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="N30" t="s">
+      <c r="N30" t="s" s="0">
         <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31">
+      <c r="A31" s="0">
         <v>31</v>
       </c>
-      <c r="C31" t="str">
+      <c r="C31" t="str" s="0">
         <f>Helper!D16</f>
         <v>Badger Bat</v>
       </c>
-      <c r="O31" t="str">
+      <c r="O31" t="str" s="0">
         <f>Helper!D49</f>
         <v>Dung Beetle</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32">
+      <c r="A32" s="0">
         <v>32</v>
       </c>
-      <c r="H32" t="s">
+      <c r="H32" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="I32" t="s">
+      <c r="I32" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="J32" t="s">
+      <c r="J32" t="s" s="0">
         <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A33">
+      <c r="A33" s="0">
         <v>33</v>
       </c>
-      <c r="C33" t="str">
+      <c r="C33" t="str" s="0">
         <f>Helper!D18</f>
         <v>Sea Otter</v>
       </c>
-      <c r="O33" t="str">
+      <c r="O33" t="str" s="0">
         <f>Helper!D51</f>
         <v>Emperor Penguin</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A34">
+      <c r="A34" s="0">
         <v>34</v>
       </c>
-      <c r="B34" t="str">
+      <c r="B34" t="str" s="0">
         <f>Helper!A2</f>
         <v>Bumblebee Bat</v>
       </c>
-      <c r="D34" t="s">
-        <v>4</v>
-      </c>
-      <c r="N34" t="s">
+      <c r="D34" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="N34" t="s" s="0">
         <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A35">
+      <c r="A35" s="0">
         <v>35</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="O35" t="str">
+      <c r="O35" t="str" s="0">
         <f>Helper!D66</f>
         <v>Lined Seahorse</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A36">
+      <c r="A36" s="0">
         <v>36</v>
       </c>
-      <c r="B36" t="str">
+      <c r="B36" t="str" s="0">
         <f>Helper!A3</f>
         <v>Shrew Mole</v>
       </c>
-      <c r="E36" t="s">
-        <v>4</v>
-      </c>
-      <c r="M36" t="s">
+      <c r="E36" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="M36" t="s" s="0">
         <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A37">
+      <c r="A37" s="0">
         <v>37</v>
       </c>
-      <c r="C37" t="str">
+      <c r="C37" t="str" s="0">
         <f>Helper!D25</f>
         <v>Southern Ningaui</v>
       </c>
-      <c r="O37" t="str">
+      <c r="O37" t="str" s="0">
         <f>Helper!D58</f>
         <v>Owl Monkey</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A38">
+      <c r="A38" s="0">
         <v>38</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="N38" t="s">
+      <c r="N38" t="s" s="0">
         <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A39">
+      <c r="A39" s="0">
         <v>39</v>
       </c>
-      <c r="C39" t="str">
+      <c r="C39" t="str" s="0">
         <f>Helper!D26</f>
         <v>Grasshopper Mouse</v>
       </c>
-      <c r="O39" t="str">
+      <c r="O39" t="str" s="0">
         <f>Helper!D59</f>
         <v>Caspian Terns</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A40">
+      <c r="A40" s="0">
         <v>40</v>
       </c>
-      <c r="F40" t="s">
-        <v>4</v>
-      </c>
-      <c r="L40" t="s">
+      <c r="F40" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="L40" t="s" s="0">
         <v>4</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A41">
+      <c r="A41" s="0">
         <v>41</v>
       </c>
-      <c r="C41" t="str">
+      <c r="C41" t="str" s="0">
         <f>Helper!D22</f>
         <v>Sibree Dwarf Lemur</v>
       </c>
-      <c r="O41" t="str">
+      <c r="O41" t="str" s="0">
         <f>Helper!D55</f>
         <v>Pacific Spiny Lumpsucker</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A42">
+      <c r="A42" s="0">
         <v>42</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="N42" t="s">
+      <c r="N42" t="s" s="0">
         <v>6</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A43">
+      <c r="A43" s="0">
         <v>43</v>
       </c>
-      <c r="C43" t="str">
+      <c r="C43" t="str" s="0">
         <f>Helper!D29</f>
         <v>Silver Pika</v>
       </c>
-      <c r="O43" t="str">
+      <c r="O43" t="str" s="0">
         <f>Helper!D62</f>
         <v>Peacock Wrasse</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A44">
+      <c r="A44" s="0">
         <v>44</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E44" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="M44" t="s">
+      <c r="M44" t="s" s="0">
         <v>7</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A45">
+      <c r="A45" s="0">
         <v>45</v>
       </c>
-      <c r="C45" t="str">
+      <c r="C45" t="str" s="0">
         <f>Helper!D21</f>
         <v>Mara</v>
       </c>
-      <c r="O45" t="str">
+      <c r="O45" t="str" s="0">
         <f>Helper!D54</f>
         <v>Siamang</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A46">
+      <c r="A46" s="0">
         <v>46</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D46" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="N46" t="s">
+      <c r="N46" t="s" s="0">
         <v>7</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A47">
+      <c r="A47" s="0">
         <v>47</v>
       </c>
-      <c r="C47" t="str">
+      <c r="C47" t="str" s="0">
         <f>Helper!D30</f>
         <v>Siberian Chipmunk</v>
       </c>
-      <c r="O47" t="str">
+      <c r="O47" t="str" s="0">
         <f>Helper!D63</f>
         <v>Darwin's Frogs</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A48">
+      <c r="A48" s="0">
         <v>48</v>
       </c>
-      <c r="G48" t="s">
-        <v>4</v>
-      </c>
-      <c r="K48" t="s">
+      <c r="G48" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="K48" t="s" s="0">
         <v>4</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A49">
+      <c r="A49" s="0">
         <v>49</v>
       </c>
-      <c r="C49" t="str">
+      <c r="C49" t="str" s="0">
         <f>Helper!D23</f>
         <v>Itjaritjari</v>
       </c>
-      <c r="O49" t="str">
+      <c r="O49" t="str" s="0">
         <f>Helper!D56</f>
         <v>Bat-Eared Fox</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A50">
+      <c r="A50" s="0">
         <v>50</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D50" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="N50" t="s">
+      <c r="N50" t="s" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A51">
+      <c r="A51" s="0">
         <v>51</v>
       </c>
-      <c r="C51" t="str">
+      <c r="C51" t="str" s="0">
         <f>Helper!D28</f>
         <v>Silky Anteater</v>
       </c>
-      <c r="O51" t="str">
+      <c r="O51" t="str" s="0">
         <f>Helper!D61</f>
         <v>Spotted sandpiper</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A52">
+      <c r="A52" s="0">
         <v>52</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E52" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="M52" t="s">
+      <c r="M52" t="s" s="0">
         <v>9</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A53">
+      <c r="A53" s="0">
         <v>53</v>
       </c>
-      <c r="C53" t="str">
+      <c r="C53" t="str" s="0">
         <f>Helper!D20</f>
         <v>Dik Dik</v>
       </c>
-      <c r="O53" t="str">
+      <c r="O53" t="str" s="0">
         <f>Helper!D53</f>
         <v>Wolverine</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A54">
+      <c r="A54" s="0">
         <v>54</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D54" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="N54" t="s">
+      <c r="N54" t="s" s="0">
         <v>9</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A55">
+      <c r="A55" s="0">
         <v>55</v>
       </c>
-      <c r="C55" t="str">
+      <c r="C55" t="str" s="0">
         <f>Helper!D31</f>
         <v>Colo Colo Opossum</v>
       </c>
-      <c r="O55" t="str">
+      <c r="O55" t="str" s="0">
         <f>Helper!D64</f>
         <v>Giant Water Bug</v>
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A56">
+      <c r="A56" s="0">
         <v>56</v>
       </c>
-      <c r="F56" t="s">
+      <c r="F56" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="L56" t="s">
+      <c r="L56" t="s" s="0">
         <v>11</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A57">
+      <c r="A57" s="0">
         <v>57</v>
       </c>
-      <c r="C57" t="str">
+      <c r="C57" t="str" s="0">
         <f>Helper!D24</f>
         <v>Bulldog Bat</v>
       </c>
-      <c r="O57" t="str">
+      <c r="O57" t="str" s="0">
         <f>Helper!D57</f>
         <v>Greater Flamingo</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A58">
+      <c r="A58" s="0">
         <v>58</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D58" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="N58" t="s">
+      <c r="N58" t="s" s="0">
         <v>10</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A59">
+      <c r="A59" s="0">
         <v>59</v>
       </c>
-      <c r="C59" t="str">
+      <c r="C59" t="str" s="0">
         <f>Helper!D27</f>
         <v>Thor's Hero Shrew</v>
       </c>
-      <c r="O59" t="str">
+      <c r="O59" t="str" s="0">
         <f>Helper!D60</f>
         <v>Dyak Fruit Bat</v>
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A60">
+      <c r="A60" s="0">
         <v>60</v>
       </c>
-      <c r="E60" t="s">
+      <c r="E60" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="M60" t="s">
+      <c r="M60" t="s" s="0">
         <v>11</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A61">
+      <c r="A61" s="0">
         <v>61</v>
       </c>
-      <c r="C61" t="str">
+      <c r="C61" t="str" s="0">
         <f>Helper!D19</f>
         <v xml:space="preserve">Rock Hyrax </v>
       </c>
-      <c r="O61" t="str">
+      <c r="O61" t="str" s="0">
         <f>Helper!D52</f>
         <v>Greater Rhea</v>
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A62">
+      <c r="A62" s="0">
         <v>62</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D62" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="N62" t="s">
+      <c r="N62" t="s" s="0">
         <v>11</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A63">
+      <c r="A63" s="0">
         <v>63</v>
       </c>
-      <c r="C63" t="str">
+      <c r="C63" t="str" s="0">
         <f>Helper!D32</f>
         <v>Pygmy Jerboa</v>
       </c>
-      <c r="O63" t="str">
+      <c r="O63" t="str" s="0">
         <f>Helper!D65</f>
         <v xml:space="preserve">Three-Spined stickleback </v>
       </c>
@@ -2572,773 +2669,773 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
-    <col min="3" max="15" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="14.7109375"/>
+    <col min="3" max="15" customWidth="true" width="23.7109375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1">
+      <c r="A1" s="0">
         <v>0</v>
       </c>
-      <c r="C1" t="str">
+      <c r="C1" t="str" s="0">
         <f>Helper!D2</f>
         <v>Okapi</v>
       </c>
-      <c r="O1" t="str">
+      <c r="O1" t="str" s="0">
         <f>Helper!D35</f>
         <v>Golden Eagle</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="0">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" t="s" s="0">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="0">
         <v>2</v>
       </c>
-      <c r="C3" t="str">
+      <c r="C3" t="str" s="0">
         <f>Helper!D17</f>
         <v>Four-Striped Grass Mouse</v>
       </c>
-      <c r="O3" t="str">
+      <c r="O3" t="str" s="0">
         <f>Helper!D50</f>
         <v>Spongilla Fly</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="0">
         <v>3</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4" t="s" s="0">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="C5" t="str">
+      <c r="A5" s="0">
+        <v>4</v>
+      </c>
+      <c r="C5" t="str" s="0">
         <f>Helper!D9</f>
         <v>Striped Polecat</v>
       </c>
-      <c r="O5" t="str">
+      <c r="O5" t="str" s="0">
         <f>Helper!D42</f>
         <v>Veined Octopus</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="0">
         <v>5</v>
       </c>
-      <c r="D6" t="s">
-        <v>32</v>
-      </c>
-      <c r="N6" t="s">
-        <v>34</v>
+      <c r="D6" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="N6" t="s" s="0">
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="0">
         <v>6</v>
       </c>
-      <c r="C7" t="str">
+      <c r="C7" t="str" s="0">
         <f>Helper!D10</f>
         <v>Giant striped mongoose</v>
       </c>
-      <c r="O7" t="str">
+      <c r="O7" t="str" s="0">
         <f>Helper!D43</f>
         <v>Puffer Fish</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="0">
         <v>7</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="L8" t="s">
+      <c r="L8" t="s" s="0">
         <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="0">
         <v>8</v>
       </c>
-      <c r="C9" t="str">
+      <c r="C9" t="str" s="0">
         <f>Helper!D6</f>
         <v>Side-striped jackal</v>
       </c>
-      <c r="O9" t="str">
+      <c r="O9" t="str" s="0">
         <f>Helper!D39</f>
         <v>Palaeocastor</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" s="0">
         <v>9</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="N10" t="s">
-        <v>35</v>
+      <c r="N10" t="s" s="0">
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="0">
         <v>10</v>
       </c>
-      <c r="C11" t="str">
+      <c r="C11" t="str" s="0">
         <f>Helper!D13</f>
         <v>Striped Possum</v>
       </c>
-      <c r="O11" t="str">
+      <c r="O11" t="str" s="0">
         <f>Helper!D46</f>
         <v>Trapdoor Spider</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="0">
         <v>11</v>
       </c>
-      <c r="E12" t="s">
-        <v>44</v>
-      </c>
-      <c r="M12" t="s">
+      <c r="E12" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="M12" t="s" s="0">
         <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" s="0">
         <v>12</v>
       </c>
-      <c r="C13" t="str">
+      <c r="C13" t="str" s="0">
         <f>Helper!D5</f>
         <v>Striped dolphin</v>
       </c>
-      <c r="O13" t="str">
+      <c r="O13" t="str" s="0">
         <f>Helper!D38</f>
         <v>Lungfish</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="A14" s="0">
         <v>13</v>
       </c>
-      <c r="D14" t="s">
-        <v>44</v>
-      </c>
-      <c r="N14" t="s">
+      <c r="D14" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="N14" t="s" s="0">
         <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="A15" s="0">
         <v>14</v>
       </c>
-      <c r="C15" t="str">
+      <c r="C15" t="str" s="0">
         <f>Helper!D14</f>
         <v>Chequered elephant shrew</v>
       </c>
-      <c r="O15" t="str">
+      <c r="O15" t="str" s="0">
         <f>Helper!D47</f>
         <v>Tent-making Bat</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="A16" s="0">
         <v>15</v>
       </c>
-      <c r="G16" t="s">
-        <v>19</v>
-      </c>
-      <c r="K16" t="s">
+      <c r="G16" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="K16" t="s" s="0">
         <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="A17" s="0">
         <v>16</v>
       </c>
-      <c r="C17" t="str">
+      <c r="C17" t="str" s="0">
         <f>Helper!D7</f>
         <v>Wildcat</v>
       </c>
-      <c r="O17" t="str">
+      <c r="O17" t="str" s="0">
         <f>Helper!D40</f>
         <v>Goanna</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="A18" s="0">
         <v>17</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="N18" t="s">
+      <c r="N18" t="s" s="0">
         <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="A19" s="0">
         <v>18</v>
       </c>
-      <c r="C19" t="str">
+      <c r="C19" t="str" s="0">
         <f>Helper!D12</f>
         <v>Highland Streaked Tenrec</v>
       </c>
-      <c r="O19" t="str">
+      <c r="O19" t="str" s="0">
         <f>Helper!D45</f>
         <v>Rufous Hornero</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="A20" s="0">
         <v>19</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="M20" t="s">
+      <c r="M20" t="s" s="0">
         <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="A21" s="0">
         <v>20</v>
       </c>
-      <c r="C21" t="str">
+      <c r="C21" t="str" s="0">
         <f>Helper!D4</f>
         <v>Striped hyena</v>
       </c>
-      <c r="O21" t="str">
+      <c r="O21" t="str" s="0">
         <f>Helper!D37</f>
         <v>Homo habilis</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="A22" s="0">
         <v>21</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="N22" t="s">
+      <c r="N22" t="s" s="0">
         <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="A23" s="0">
         <v>22</v>
       </c>
-      <c r="C23" t="str">
+      <c r="C23" t="str" s="0">
         <f>Helper!D15</f>
         <v>Fire-footed Rope Squirrel</v>
       </c>
-      <c r="O23" t="str">
+      <c r="O23" t="str" s="0">
         <f>Helper!D48</f>
         <v>Bee</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24">
+      <c r="A24" s="0">
         <v>23</v>
       </c>
-      <c r="F24" t="s">
-        <v>19</v>
-      </c>
-      <c r="L24" t="s">
-        <v>23</v>
+      <c r="F24" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="L24" t="s" s="0">
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25">
+      <c r="A25" s="0">
         <v>24</v>
       </c>
-      <c r="C25" t="str">
+      <c r="C25" t="str" s="0">
         <f>Helper!D8</f>
         <v>Striped Rabbit</v>
       </c>
-      <c r="O25" t="str">
+      <c r="O25" t="str" s="0">
         <f>Helper!D41</f>
         <v>Montezuma Oropendola</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26">
+      <c r="A26" s="0">
         <v>25</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" t="s" s="0">
         <v>27</v>
       </c>
-      <c r="N26" t="s">
-        <v>29</v>
+      <c r="N26" t="s" s="0">
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27">
+      <c r="A27" s="0">
         <v>26</v>
       </c>
-      <c r="C27" t="str">
+      <c r="C27" t="str" s="0">
         <f>Helper!D11</f>
         <v>Numbat</v>
       </c>
-      <c r="O27" t="str">
+      <c r="O27" t="str" s="0">
         <f>Helper!D44</f>
         <v>New Caledonian Crow</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28">
+      <c r="A28" s="0">
         <v>27</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" t="s" s="0">
         <v>27</v>
       </c>
-      <c r="M28" t="s">
-        <v>23</v>
+      <c r="M28" t="s" s="0">
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29">
+      <c r="A29" s="0">
         <v>28</v>
       </c>
-      <c r="C29" t="str">
+      <c r="C29" t="str" s="0">
         <f>Helper!D3</f>
         <v>Kudu</v>
       </c>
-      <c r="O29" t="str">
+      <c r="O29" t="str" s="0">
         <f>Helper!D36</f>
         <v>Cathedral Termite</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30">
+      <c r="A30" s="0">
         <v>29</v>
       </c>
-      <c r="D30" t="s">
-        <v>45</v>
-      </c>
-      <c r="N30" t="s">
+      <c r="D30" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="N30" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31">
+      <c r="A31" s="0">
         <v>30</v>
       </c>
-      <c r="C31" t="str">
+      <c r="C31" t="str" s="0">
         <f>Helper!D16</f>
         <v>Badger Bat</v>
       </c>
-      <c r="O31" t="str">
+      <c r="O31" t="str" s="0">
         <f>Helper!D49</f>
         <v>Dung Beetle</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32">
+      <c r="A32" s="0">
         <v>31</v>
       </c>
-      <c r="H32" t="s">
-        <v>30</v>
-      </c>
-      <c r="I32" t="s">
+      <c r="H32" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="I32" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="J32" t="s" s="0">
         <v>21</v>
       </c>
-      <c r="J32" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A33">
+      <c r="A33" s="0">
         <v>32</v>
       </c>
-      <c r="C33" t="str">
+      <c r="C33" t="str" s="0">
         <f>Helper!D18</f>
         <v>Sea Otter</v>
       </c>
-      <c r="O33" t="str">
+      <c r="O33" t="str" s="0">
         <f>Helper!D51</f>
         <v>Emperor Penguin</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A34">
+      <c r="A34" s="0">
         <v>33</v>
       </c>
-      <c r="B34" t="str">
+      <c r="B34" t="str" s="0">
         <f>Helper!A2</f>
         <v>Bumblebee Bat</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" t="s" s="0">
         <v>41</v>
       </c>
-      <c r="N34" t="s">
+      <c r="N34" t="s" s="0">
         <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A35">
+      <c r="A35" s="0">
         <v>34</v>
       </c>
-      <c r="C35" t="s">
-        <v>43</v>
-      </c>
-      <c r="O35" t="str">
+      <c r="C35" t="s" s="0">
+        <v>59</v>
+      </c>
+      <c r="O35" t="str" s="0">
         <f>Helper!D66</f>
         <v>Lined Seahorse</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A36">
+      <c r="A36" s="0">
         <v>35</v>
       </c>
-      <c r="B36" t="str">
+      <c r="B36" t="str" s="0">
         <f>Helper!A3</f>
         <v>Shrew Mole</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36" t="s" s="0">
         <v>41</v>
       </c>
-      <c r="M36" t="s">
+      <c r="M36" t="s" s="0">
         <v>24</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A37">
+      <c r="A37" s="0">
         <v>36</v>
       </c>
-      <c r="C37" t="str">
+      <c r="C37" t="str" s="0">
         <f>Helper!D25</f>
         <v>Southern Ningaui</v>
       </c>
-      <c r="O37" t="str">
+      <c r="O37" t="str" s="0">
         <f>Helper!D58</f>
         <v>Owl Monkey</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A38">
+      <c r="A38" s="0">
         <v>37</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" t="s" s="0">
         <v>46</v>
       </c>
-      <c r="N38" t="s">
+      <c r="N38" t="s" s="0">
         <v>25</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A39">
+      <c r="A39" s="0">
         <v>38</v>
       </c>
-      <c r="C39" t="str">
+      <c r="C39" t="str" s="0">
         <f>Helper!D26</f>
         <v>Grasshopper Mouse</v>
       </c>
-      <c r="O39" t="str">
+      <c r="O39" t="str" s="0">
         <f>Helper!D59</f>
         <v>Caspian Terns</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A40">
+      <c r="A40" s="0">
         <v>39</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F40" t="s" s="0">
         <v>41</v>
       </c>
-      <c r="L40" t="s">
+      <c r="L40" t="s" s="0">
         <v>24</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A41">
+      <c r="A41" s="0">
         <v>40</v>
       </c>
-      <c r="C41" t="str">
+      <c r="C41" t="str" s="0">
         <f>Helper!D22</f>
         <v>Sibree Dwarf Lemur</v>
       </c>
-      <c r="O41" t="str">
+      <c r="O41" t="str" s="0">
         <f>Helper!D55</f>
         <v>Pacific Spiny Lumpsucker</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A42">
+      <c r="A42" s="0">
         <v>41</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="N42" t="s">
+      <c r="N42" t="s" s="0">
         <v>38</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A43">
+      <c r="A43" s="0">
         <v>42</v>
       </c>
-      <c r="C43" t="str">
+      <c r="C43" t="str" s="0">
         <f>Helper!D29</f>
         <v>Silver Pika</v>
       </c>
-      <c r="O43" t="str">
+      <c r="O43" t="str" s="0">
         <f>Helper!D62</f>
         <v>Peacock Wrasse</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A44">
+      <c r="A44" s="0">
         <v>43</v>
       </c>
-      <c r="E44" t="s">
-        <v>37</v>
-      </c>
-      <c r="M44" t="s">
+      <c r="E44" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="M44" t="s" s="0">
         <v>26</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A45">
+      <c r="A45" s="0">
         <v>44</v>
       </c>
-      <c r="C45" t="str">
+      <c r="C45" t="str" s="0">
         <f>Helper!D21</f>
         <v>Mara</v>
       </c>
-      <c r="O45" t="str">
+      <c r="O45" t="str" s="0">
         <f>Helper!D54</f>
         <v>Siamang</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A46">
+      <c r="A46" s="0">
         <v>45</v>
       </c>
-      <c r="D46" t="s">
-        <v>47</v>
-      </c>
-      <c r="N46" t="s">
+      <c r="D46" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="N46" t="s" s="0">
         <v>26</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A47">
+      <c r="A47" s="0">
         <v>46</v>
       </c>
-      <c r="C47" t="str">
+      <c r="C47" t="str" s="0">
         <f>Helper!D30</f>
         <v>Siberian Chipmunk</v>
       </c>
-      <c r="O47" t="str">
+      <c r="O47" t="str" s="0">
         <f>Helper!D63</f>
         <v>Darwin's Frogs</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A48">
+      <c r="A48" s="0">
         <v>47</v>
       </c>
-      <c r="G48" t="s">
-        <v>30</v>
-      </c>
-      <c r="K48" t="s">
-        <v>31</v>
+      <c r="G48" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="K48" t="s" s="0">
+        <v>24</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A49">
+      <c r="A49" s="0">
         <v>48</v>
       </c>
-      <c r="C49" t="str">
+      <c r="C49" t="str" s="0">
         <f>Helper!D23</f>
         <v>Itjaritjari</v>
       </c>
-      <c r="O49" t="str">
+      <c r="O49" t="str" s="0">
         <f>Helper!D56</f>
         <v>Bat-Eared Fox</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A50">
+      <c r="A50" s="0">
         <v>49</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D50" t="s" s="0">
         <v>48</v>
       </c>
-      <c r="N50" t="s">
-        <v>39</v>
+      <c r="N50" t="s" s="0">
+        <v>55</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A51">
+      <c r="A51" s="0">
         <v>50</v>
       </c>
-      <c r="C51" t="str">
+      <c r="C51" t="str" s="0">
         <f>Helper!D28</f>
         <v>Silky Anteater</v>
       </c>
-      <c r="O51" t="str">
+      <c r="O51" t="str" s="0">
         <f>Helper!D61</f>
         <v>Spotted sandpiper</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A52">
+      <c r="A52" s="0">
         <v>51</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E52" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="M52" t="s">
+      <c r="M52" t="s" s="0">
         <v>31</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A53">
+      <c r="A53" s="0">
         <v>52</v>
       </c>
-      <c r="C53" t="str">
+      <c r="C53" t="str" s="0">
         <f>Helper!D20</f>
         <v>Dik Dik</v>
       </c>
-      <c r="O53" t="str">
+      <c r="O53" t="str" s="0">
         <f>Helper!D53</f>
         <v>Wolverine</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A54">
+      <c r="A54" s="0">
         <v>53</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D54" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="N54" t="s">
+      <c r="N54" t="s" s="0">
         <v>31</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A55">
+      <c r="A55" s="0">
         <v>54</v>
       </c>
-      <c r="C55" t="str">
+      <c r="C55" t="str" s="0">
         <f>Helper!D31</f>
         <v>Colo Colo Opossum</v>
       </c>
-      <c r="O55" t="str">
+      <c r="O55" t="str" s="0">
         <f>Helper!D64</f>
         <v>Giant Water Bug</v>
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A56">
+      <c r="A56" s="0">
         <v>55</v>
       </c>
-      <c r="F56" t="s">
-        <v>30</v>
-      </c>
-      <c r="L56" t="s">
-        <v>31</v>
+      <c r="F56" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="L56" t="s" s="0">
+        <v>28</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A57">
+      <c r="A57" s="0">
         <v>56</v>
       </c>
-      <c r="C57" t="str">
+      <c r="C57" t="str" s="0">
         <f>Helper!D24</f>
         <v>Bulldog Bat</v>
       </c>
-      <c r="O57" t="str">
+      <c r="O57" t="str" s="0">
         <f>Helper!D57</f>
         <v>Greater Flamingo</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A58">
+      <c r="A58" s="0">
         <v>57</v>
       </c>
-      <c r="D58" t="s">
-        <v>33</v>
-      </c>
-      <c r="N58" t="s">
+      <c r="D58" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="N58" t="s" s="0">
         <v>40</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A59">
+      <c r="A59" s="0">
         <v>58</v>
       </c>
-      <c r="C59" t="str">
+      <c r="C59" t="str" s="0">
         <f>Helper!D27</f>
         <v>Thor's Hero Shrew</v>
       </c>
-      <c r="O59" t="str">
+      <c r="O59" t="str" s="0">
         <f>Helper!D60</f>
         <v>Dyak Fruit Bat</v>
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A60">
+      <c r="A60" s="0">
         <v>59</v>
       </c>
-      <c r="E60" t="s">
+      <c r="E60" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="M60" t="s">
-        <v>40</v>
+      <c r="M60" t="s" s="0">
+        <v>28</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A61">
+      <c r="A61" s="0">
         <v>60</v>
       </c>
-      <c r="C61" t="str">
+      <c r="C61" t="str" s="0">
         <f>Helper!D19</f>
         <v xml:space="preserve">Rock Hyrax </v>
       </c>
-      <c r="O61" t="str">
+      <c r="O61" t="str" s="0">
         <f>Helper!D52</f>
         <v>Greater Rhea</v>
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A62">
+      <c r="A62" s="0">
         <v>61</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D62" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="N62" t="s">
+      <c r="N62" t="s" s="0">
         <v>28</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A63">
+      <c r="A63" s="0">
         <v>62</v>
       </c>
-      <c r="C63" t="str">
+      <c r="C63" t="str" s="0">
         <f>Helper!D32</f>
         <v>Pygmy Jerboa</v>
       </c>
-      <c r="O63" t="str">
+      <c r="O63" t="str" s="0">
         <f>Helper!D65</f>
         <v xml:space="preserve">Three-Spined stickleback </v>
       </c>

</xml_diff>

<commit_message>
Debugged code so now it work properly. Next add the GUI
</commit_message>
<xml_diff>
--- a/Resources/Bracket.xlsx
+++ b/Resources/Bracket.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pants\IdeaProjects\Mam\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22691597-4C72-4998-867E-40D08655AFBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{814F9D21-F62F-4EEB-922D-8204F3C797E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8928" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Helper" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6341" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1602" uniqueCount="81">
   <si>
     <t>Type in the two Wildcard animals below</t>
   </si>
@@ -91,196 +91,196 @@
     <t>Okapi</t>
   </si>
   <si>
+    <t>Striped hyena</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rock Hyrax </t>
+  </si>
+  <si>
+    <t>Golden Eagle</t>
+  </si>
+  <si>
+    <t>Homo habilis</t>
+  </si>
+  <si>
+    <t>Cathedral Termite</t>
+  </si>
+  <si>
+    <t>Emperor Penguin</t>
+  </si>
+  <si>
+    <t>Owl Monkey</t>
+  </si>
+  <si>
+    <t>Siamang</t>
+  </si>
+  <si>
+    <t>Striped Rabbit</t>
+  </si>
+  <si>
+    <t>Greater Rhea</t>
+  </si>
+  <si>
+    <t>Dik Dik</t>
+  </si>
+  <si>
+    <t>Wolverine</t>
+  </si>
+  <si>
+    <t>Greater Flamingo</t>
+  </si>
+  <si>
+    <t>Sea Otter</t>
+  </si>
+  <si>
+    <t>Lungfish</t>
+  </si>
+  <si>
+    <t>Southern Ningaui</t>
+  </si>
+  <si>
+    <t>Itjaritjari</t>
+  </si>
+  <si>
+    <t>Striped dolphin</t>
+  </si>
+  <si>
+    <t>Kudu</t>
+  </si>
+  <si>
+    <t>Mara</t>
+  </si>
+  <si>
+    <t>Bat-Eared Fox</t>
+  </si>
+  <si>
+    <t>Bulldog Bat</t>
+  </si>
+  <si>
+    <t>Shrew Mole</t>
+  </si>
+  <si>
+    <t>Veined Octopus</t>
+  </si>
+  <si>
+    <t>Palaeocastor</t>
+  </si>
+  <si>
+    <t>Highland Streaked Tenrec</t>
+  </si>
+  <si>
+    <t>Rufous Hornero</t>
+  </si>
+  <si>
+    <t>Montezuma Oropendola</t>
+  </si>
+  <si>
+    <t>Peacock Wrasse</t>
+  </si>
+  <si>
+    <t>Giant striped mongoose</t>
+  </si>
+  <si>
+    <t>Striped Possum</t>
+  </si>
+  <si>
+    <t>Silver Pika</t>
+  </si>
+  <si>
+    <t>Bumblebee Bat</t>
+  </si>
+  <si>
     <t>Side-striped jackal</t>
   </si>
   <si>
     <t>Wildcat</t>
   </si>
   <si>
-    <t>Striped hyena</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rock Hyrax </t>
-  </si>
-  <si>
-    <t>Golden Eagle</t>
-  </si>
-  <si>
-    <t>Homo habilis</t>
-  </si>
-  <si>
-    <t>Cathedral Termite</t>
-  </si>
-  <si>
-    <t>Emperor Penguin</t>
-  </si>
-  <si>
-    <t>Owl Monkey</t>
-  </si>
-  <si>
-    <t>Siamang</t>
-  </si>
-  <si>
-    <t>Striped Rabbit</t>
-  </si>
-  <si>
-    <t>Greater Rhea</t>
-  </si>
-  <si>
-    <t>Montezuma Oropendola</t>
-  </si>
-  <si>
-    <t>Dik Dik</t>
-  </si>
-  <si>
-    <t>Wolverine</t>
-  </si>
-  <si>
-    <t>Giant striped mongoose</t>
+    <t>Fire-footed Rope Squirrel</t>
+  </si>
+  <si>
+    <t>Grasshopper Mouse</t>
+  </si>
+  <si>
+    <t>Sibree Dwarf Lemur</t>
+  </si>
+  <si>
+    <t>Puffer Fish</t>
+  </si>
+  <si>
+    <t>New Caledonian Crow</t>
+  </si>
+  <si>
+    <t>Caspian Terns</t>
+  </si>
+  <si>
+    <t>Pacific Spiny Lumpsucker</t>
+  </si>
+  <si>
+    <t>Darwin's Frogs</t>
+  </si>
+  <si>
+    <t>Spotted sandpiper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Three-Spined stickleback </t>
+  </si>
+  <si>
+    <t>Siberian Chipmunk</t>
+  </si>
+  <si>
+    <t>Silky Anteater</t>
   </si>
   <si>
     <t>Thor's Hero Shrew</t>
   </si>
   <si>
-    <t>Veined Octopus</t>
-  </si>
-  <si>
-    <t>Palaeocastor</t>
+    <t>Trapdoor Spider</t>
   </si>
   <si>
     <t>Goanna</t>
   </si>
   <si>
-    <t>Sibree Dwarf Lemur</t>
-  </si>
-  <si>
-    <t>Pacific Spiny Lumpsucker</t>
-  </si>
-  <si>
-    <t>Spotted sandpiper</t>
-  </si>
-  <si>
-    <t>Greater Flamingo</t>
-  </si>
-  <si>
-    <t>Sea Otter</t>
-  </si>
-  <si>
-    <t>Lungfish</t>
-  </si>
-  <si>
-    <t>Bumblebee Bat</t>
+    <t>Striped Polecat</t>
   </si>
   <si>
     <t>Chequered elephant shrew</t>
   </si>
   <si>
+    <t>Pygmy Jerboa</t>
+  </si>
+  <si>
+    <t>Tent-making Bat</t>
+  </si>
+  <si>
+    <t>Numbat</t>
+  </si>
+  <si>
+    <t>Bee</t>
+  </si>
+  <si>
+    <t>Lined Seahorse</t>
+  </si>
+  <si>
+    <t>Dyak Fruit Bat</t>
+  </si>
+  <si>
+    <t>Giant Water Bug</t>
+  </si>
+  <si>
+    <t>Four-Striped Grass Mouse</t>
+  </si>
+  <si>
+    <t>Colo Colo Opossum</t>
+  </si>
+  <si>
     <t>Badger Bat</t>
   </si>
   <si>
-    <t>Southern Ningaui</t>
-  </si>
-  <si>
-    <t>Siberian Chipmunk</t>
-  </si>
-  <si>
-    <t>Itjaritjari</t>
-  </si>
-  <si>
-    <t>Striped dolphin</t>
-  </si>
-  <si>
-    <t>New Caledonian Crow</t>
-  </si>
-  <si>
-    <t>Kudu</t>
-  </si>
-  <si>
-    <t>Silver Pika</t>
-  </si>
-  <si>
-    <t>Peacock Wrasse</t>
-  </si>
-  <si>
-    <t>Mara</t>
-  </si>
-  <si>
-    <t>Bat-Eared Fox</t>
-  </si>
-  <si>
-    <t>Colo Colo Opossum</t>
-  </si>
-  <si>
-    <t>Giant Water Bug</t>
-  </si>
-  <si>
-    <t>Bulldog Bat</t>
-  </si>
-  <si>
-    <t>Shrew Mole</t>
-  </si>
-  <si>
-    <t>Puffer Fish</t>
-  </si>
-  <si>
-    <t>Trapdoor Spider</t>
-  </si>
-  <si>
-    <t>Highland Streaked Tenrec</t>
-  </si>
-  <si>
-    <t>Rufous Hornero</t>
-  </si>
-  <si>
-    <t>Silky Anteater</t>
-  </si>
-  <si>
-    <t>Pygmy Jerboa</t>
-  </si>
-  <si>
-    <t>Striped Polecat</t>
-  </si>
-  <si>
-    <t>Bee</t>
-  </si>
-  <si>
-    <t>Grasshopper Mouse</t>
-  </si>
-  <si>
-    <t>Caspian Terns</t>
-  </si>
-  <si>
-    <t>Dyak Fruit Bat</t>
-  </si>
-  <si>
-    <t>Striped Possum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Three-Spined stickleback </t>
-  </si>
-  <si>
-    <t>Numbat</t>
-  </si>
-  <si>
-    <t>Four-Striped Grass Mouse</t>
-  </si>
-  <si>
-    <t>Lined Seahorse</t>
-  </si>
-  <si>
     <t>Dung Beetle</t>
   </si>
   <si>
-    <t>Fire-footed Rope Squirrel</t>
-  </si>
-  <si>
-    <t>Tent-making Bat</t>
-  </si>
-  <si>
     <t>Spongilla Fly</t>
-  </si>
-  <si>
-    <t>Darwin's Frogs</t>
   </si>
 </sst>
 </file>
@@ -987,15 +987,15 @@
       <selection activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="36.140625"/>
-    <col min="2" max="2" customWidth="true" width="41.28515625"/>
-    <col min="3" max="3" customWidth="true" width="18.42578125"/>
+    <col min="1" max="1" customWidth="true" width="36.109375"/>
+    <col min="2" max="2" customWidth="true" width="41.33203125"/>
+    <col min="3" max="3" customWidth="true" width="18.44140625"/>
     <col min="4" max="4" customWidth="true" width="25.0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1009,7 +1009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="str">
         <f>[1]Sheet1!C17</f>
         <v>Bumblebee Bat</v>
@@ -1025,7 +1025,7 @@
         <v>Okapi</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="str">
         <f>[1]Sheet1!C18</f>
         <v>Shrew Mole</v>
@@ -1041,7 +1041,7 @@
         <v>Kudu</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1">
         <v>1</v>
@@ -1054,7 +1054,7 @@
         <v>Striped hyena</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1">
         <v>1</v>
@@ -1067,7 +1067,7 @@
         <v>Striped dolphin</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1">
         <v>1</v>
@@ -1080,7 +1080,7 @@
         <v>Side-striped jackal</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1">
         <v>1</v>
@@ -1093,7 +1093,7 @@
         <v>Wildcat</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1">
         <v>1</v>
@@ -1106,7 +1106,7 @@
         <v>Striped Rabbit</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1">
         <v>1</v>
@@ -1119,7 +1119,7 @@
         <v>Striped Polecat</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1">
         <v>1</v>
@@ -1132,7 +1132,7 @@
         <v>Giant striped mongoose</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1">
         <v>1</v>
@@ -1145,7 +1145,7 @@
         <v>Numbat</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1">
         <v>1</v>
@@ -1158,7 +1158,7 @@
         <v>Highland Streaked Tenrec</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1">
         <v>1</v>
@@ -1171,7 +1171,7 @@
         <v>Striped Possum</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1">
         <v>1</v>
@@ -1184,7 +1184,7 @@
         <v>Chequered elephant shrew</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1">
         <v>1</v>
@@ -1197,7 +1197,7 @@
         <v>Fire-footed Rope Squirrel</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1">
         <v>1</v>
@@ -1210,7 +1210,7 @@
         <v>Badger Bat</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1">
         <v>1</v>
@@ -1223,7 +1223,7 @@
         <v>Four-Striped Grass Mouse</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1">
         <v>2</v>
@@ -1236,7 +1236,7 @@
         <v>Sea Otter</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1">
         <v>2</v>
@@ -1249,7 +1249,7 @@
         <v xml:space="preserve">Rock Hyrax </v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1">
         <v>2</v>
@@ -1262,7 +1262,7 @@
         <v>Dik Dik</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1">
         <v>2</v>
@@ -1275,7 +1275,7 @@
         <v>Mara</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1">
         <v>2</v>
@@ -1288,7 +1288,7 @@
         <v>Sibree Dwarf Lemur</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1">
         <v>2</v>
@@ -1301,7 +1301,7 @@
         <v>Itjaritjari</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="1">
         <v>2</v>
@@ -1314,7 +1314,7 @@
         <v>Bulldog Bat</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1">
         <v>2</v>
@@ -1327,7 +1327,7 @@
         <v>Southern Ningaui</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1">
         <v>2</v>
@@ -1340,7 +1340,7 @@
         <v>Grasshopper Mouse</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="1">
         <v>2</v>
@@ -1353,7 +1353,7 @@
         <v>Thor's Hero Shrew</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="1">
         <v>2</v>
@@ -1366,7 +1366,7 @@
         <v>Silky Anteater</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="1">
         <v>2</v>
@@ -1379,7 +1379,7 @@
         <v>Silver Pika</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="1">
         <v>2</v>
@@ -1392,7 +1392,7 @@
         <v>Siberian Chipmunk</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="1">
         <v>2</v>
@@ -1405,7 +1405,7 @@
         <v>Colo Colo Opossum</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="1">
         <v>2</v>
@@ -1418,7 +1418,7 @@
         <v>Pygmy Jerboa</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="1">
         <v>2</v>
@@ -1431,7 +1431,7 @@
         <v>Bumblebee Bat</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="1">
         <v>2</v>
@@ -1444,7 +1444,7 @@
         <v>Shrew Mole</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="1">
         <v>3</v>
@@ -1457,7 +1457,7 @@
         <v>Golden Eagle</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="1">
         <v>3</v>
@@ -1470,7 +1470,7 @@
         <v>Cathedral Termite</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="1">
         <v>3</v>
@@ -1483,7 +1483,7 @@
         <v>Homo habilis</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="1">
         <v>3</v>
@@ -1496,7 +1496,7 @@
         <v>Lungfish</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="1">
         <v>3</v>
@@ -1509,7 +1509,7 @@
         <v>Palaeocastor</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="1">
         <v>3</v>
@@ -1522,7 +1522,7 @@
         <v>Goanna</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="1">
         <v>3</v>
@@ -1535,7 +1535,7 @@
         <v>Montezuma Oropendola</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="1">
         <v>3</v>
@@ -1548,7 +1548,7 @@
         <v>Veined Octopus</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="1">
         <v>3</v>
@@ -1561,7 +1561,7 @@
         <v>Puffer Fish</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="1">
         <v>3</v>
@@ -1574,7 +1574,7 @@
         <v>New Caledonian Crow</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="1">
         <v>3</v>
@@ -1587,7 +1587,7 @@
         <v>Rufous Hornero</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
       <c r="B46" s="1">
         <v>3</v>
@@ -1600,7 +1600,7 @@
         <v>Trapdoor Spider</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="B47" s="1">
         <v>3</v>
@@ -1613,7 +1613,7 @@
         <v>Tent-making Bat</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
       <c r="B48" s="1">
         <v>3</v>
@@ -1626,7 +1626,7 @@
         <v>Bee</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
       <c r="B49" s="1">
         <v>3</v>
@@ -1639,7 +1639,7 @@
         <v>Dung Beetle</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
       <c r="B50" s="1">
         <v>3</v>
@@ -1652,7 +1652,7 @@
         <v>Spongilla Fly</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
       <c r="B51" s="1">
         <v>4</v>
@@ -1665,7 +1665,7 @@
         <v>Emperor Penguin</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
       <c r="B52" s="1">
         <v>4</v>
@@ -1678,7 +1678,7 @@
         <v>Greater Rhea</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
       <c r="B53" s="1">
         <v>4</v>
@@ -1691,7 +1691,7 @@
         <v>Wolverine</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="1"/>
       <c r="B54" s="1">
         <v>4</v>
@@ -1704,7 +1704,7 @@
         <v>Siamang</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="1"/>
       <c r="B55" s="1">
         <v>4</v>
@@ -1717,7 +1717,7 @@
         <v>Pacific Spiny Lumpsucker</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="1"/>
       <c r="B56" s="1">
         <v>4</v>
@@ -1730,7 +1730,7 @@
         <v>Bat-Eared Fox</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="1"/>
       <c r="B57" s="1">
         <v>4</v>
@@ -1743,7 +1743,7 @@
         <v>Greater Flamingo</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="1"/>
       <c r="B58" s="1">
         <v>4</v>
@@ -1756,7 +1756,7 @@
         <v>Owl Monkey</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="1"/>
       <c r="B59" s="1">
         <v>4</v>
@@ -1769,7 +1769,7 @@
         <v>Caspian Terns</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="1"/>
       <c r="B60" s="1">
         <v>4</v>
@@ -1782,7 +1782,7 @@
         <v>Dyak Fruit Bat</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="1"/>
       <c r="B61" s="1">
         <v>4</v>
@@ -1795,7 +1795,7 @@
         <v>Spotted sandpiper</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
       <c r="B62" s="1">
         <v>4</v>
@@ -1808,7 +1808,7 @@
         <v>Peacock Wrasse</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="1"/>
       <c r="B63" s="1">
         <v>4</v>
@@ -1821,7 +1821,7 @@
         <v>Darwin's Frogs</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="1"/>
       <c r="B64" s="1">
         <v>4</v>
@@ -1834,7 +1834,7 @@
         <v>Giant Water Bug</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="1"/>
       <c r="B65" s="1">
         <v>4</v>
@@ -1847,7 +1847,7 @@
         <v xml:space="preserve">Three-Spined stickleback </v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="1"/>
       <c r="B66" s="1">
         <v>4</v>
@@ -1860,7 +1860,7 @@
         <v>Lined Seahorse</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D67" s="1"/>
     </row>
   </sheetData>
@@ -1873,20 +1873,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6A13931-483F-4927-9D1A-B1180B1B7A69}">
   <dimension ref="A1:O63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="14.7109375"/>
-    <col min="3" max="3" customWidth="true" width="25.42578125"/>
-    <col min="15" max="15" customWidth="true" width="23.42578125"/>
+    <col min="2" max="2" customWidth="true" width="14.6640625"/>
+    <col min="3" max="3" customWidth="true" width="25.44140625"/>
+    <col min="15" max="15" customWidth="true" width="23.44140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" t="str" s="0">
         <f>Helper!D2</f>
@@ -1897,20 +1897,20 @@
         <v>Golden Eagle</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="0">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="N2" t="s" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="0">
         <v>2</v>
-      </c>
-      <c r="D2" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="N2" t="s" s="0">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="0">
-        <v>3</v>
       </c>
       <c r="C3" t="str" s="0">
         <f>Helper!D17</f>
@@ -1921,9 +1921,9 @@
         <v>Spongilla Fly</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="0">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E4" t="s" s="0">
         <v>4</v>
@@ -1932,9 +1932,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="0">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" t="str" s="0">
         <f>Helper!D9</f>
@@ -1945,9 +1945,9 @@
         <v>Veined Octopus</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="0">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6" t="s" s="0">
         <v>5</v>
@@ -1956,9 +1956,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="0">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" t="str" s="0">
         <f>Helper!D10</f>
@@ -1969,20 +1969,20 @@
         <v>Puffer Fish</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="0">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="L8" t="s" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" s="0">
         <v>8</v>
-      </c>
-      <c r="F8" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="L8" t="s" s="0">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="0">
-        <v>9</v>
       </c>
       <c r="C9" t="str" s="0">
         <f>Helper!D6</f>
@@ -1993,9 +1993,9 @@
         <v>Palaeocastor</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="0">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10" t="s" s="0">
         <v>6</v>
@@ -2004,9 +2004,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="0">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" t="str" s="0">
         <f>Helper!D13</f>
@@ -2017,9 +2017,9 @@
         <v>Trapdoor Spider</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="0">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E12" t="s" s="0">
         <v>7</v>
@@ -2028,9 +2028,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="0">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13" t="str" s="0">
         <f>Helper!D5</f>
@@ -2041,9 +2041,9 @@
         <v>Lungfish</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="0">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D14" t="s" s="0">
         <v>7</v>
@@ -2052,9 +2052,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="0">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15" t="str" s="0">
         <f>Helper!D14</f>
@@ -2065,20 +2065,20 @@
         <v>Tent-making Bat</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="0">
+        <v>15</v>
+      </c>
+      <c r="G16" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="K16" t="s" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A17" s="0">
         <v>16</v>
-      </c>
-      <c r="G16" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="K16" t="s" s="0">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="0">
-        <v>17</v>
       </c>
       <c r="C17" t="str" s="0">
         <f>Helper!D7</f>
@@ -2089,9 +2089,9 @@
         <v>Goanna</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="0">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D18" t="s" s="0">
         <v>8</v>
@@ -2100,9 +2100,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="0">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C19" t="str" s="0">
         <f>Helper!D12</f>
@@ -2113,9 +2113,9 @@
         <v>Rufous Hornero</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="0">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E20" t="s" s="0">
         <v>9</v>
@@ -2124,9 +2124,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="0">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C21" t="str" s="0">
         <f>Helper!D4</f>
@@ -2137,9 +2137,9 @@
         <v>Homo habilis</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="0">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D22" t="s" s="0">
         <v>9</v>
@@ -2148,9 +2148,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C23" t="str" s="0">
         <f>Helper!D15</f>
@@ -2161,9 +2161,9 @@
         <v>Bee</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="0">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F24" t="s" s="0">
         <v>11</v>
@@ -2172,9 +2172,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="0">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C25" t="str" s="0">
         <f>Helper!D8</f>
@@ -2185,9 +2185,9 @@
         <v>Montezuma Oropendola</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="0">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D26" t="s" s="0">
         <v>10</v>
@@ -2196,9 +2196,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="0">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C27" t="str" s="0">
         <f>Helper!D11</f>
@@ -2209,9 +2209,9 @@
         <v>New Caledonian Crow</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="0">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E28" t="s" s="0">
         <v>11</v>
@@ -2220,9 +2220,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="0">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C29" t="str" s="0">
         <f>Helper!D3</f>
@@ -2233,9 +2233,9 @@
         <v>Cathedral Termite</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="0">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D30" t="s" s="0">
         <v>11</v>
@@ -2244,9 +2244,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" s="0">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C31" t="str" s="0">
         <f>Helper!D16</f>
@@ -2257,9 +2257,9 @@
         <v>Dung Beetle</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="0">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H32" t="s" s="0">
         <v>13</v>
@@ -2271,9 +2271,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" s="0">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C33" t="str" s="0">
         <f>Helper!D18</f>
@@ -2284,9 +2284,9 @@
         <v>Emperor Penguin</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" s="0">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B34" t="str" s="0">
         <f>Helper!A2</f>
@@ -2299,9 +2299,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" s="0">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C35" t="s" s="0">
         <v>12</v>
@@ -2311,9 +2311,9 @@
         <v>Lined Seahorse</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" s="0">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B36" t="str" s="0">
         <f>Helper!A3</f>
@@ -2326,9 +2326,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" s="0">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C37" t="str" s="0">
         <f>Helper!D25</f>
@@ -2339,9 +2339,9 @@
         <v>Owl Monkey</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" s="0">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D38" t="s" s="0">
         <v>5</v>
@@ -2350,9 +2350,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" s="0">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C39" t="str" s="0">
         <f>Helper!D26</f>
@@ -2363,20 +2363,20 @@
         <v>Caspian Terns</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40" s="0">
+        <v>39</v>
+      </c>
+      <c r="F40" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="L40" t="s" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A41" s="0">
         <v>40</v>
-      </c>
-      <c r="F40" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="L40" t="s" s="0">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A41" s="0">
-        <v>41</v>
       </c>
       <c r="C41" t="str" s="0">
         <f>Helper!D22</f>
@@ -2387,9 +2387,9 @@
         <v>Pacific Spiny Lumpsucker</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" s="0">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D42" t="s" s="0">
         <v>6</v>
@@ -2398,9 +2398,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" s="0">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C43" t="str" s="0">
         <f>Helper!D29</f>
@@ -2411,9 +2411,9 @@
         <v>Peacock Wrasse</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" s="0">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E44" t="s" s="0">
         <v>7</v>
@@ -2422,9 +2422,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45" s="0">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C45" t="str" s="0">
         <f>Helper!D21</f>
@@ -2435,9 +2435,9 @@
         <v>Siamang</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46" s="0">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D46" t="s" s="0">
         <v>7</v>
@@ -2446,9 +2446,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" s="0">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C47" t="str" s="0">
         <f>Helper!D30</f>
@@ -2459,20 +2459,20 @@
         <v>Darwin's Frogs</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" s="0">
+        <v>47</v>
+      </c>
+      <c r="G48" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="K48" t="s" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A49" s="0">
         <v>48</v>
-      </c>
-      <c r="G48" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="K48" t="s" s="0">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A49" s="0">
-        <v>49</v>
       </c>
       <c r="C49" t="str" s="0">
         <f>Helper!D23</f>
@@ -2483,9 +2483,9 @@
         <v>Bat-Eared Fox</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50" s="0">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D50" t="s" s="0">
         <v>8</v>
@@ -2494,9 +2494,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51" s="0">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C51" t="str" s="0">
         <f>Helper!D28</f>
@@ -2507,9 +2507,9 @@
         <v>Spotted sandpiper</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52" s="0">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E52" t="s" s="0">
         <v>9</v>
@@ -2518,9 +2518,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A53" s="0">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C53" t="str" s="0">
         <f>Helper!D20</f>
@@ -2531,9 +2531,9 @@
         <v>Wolverine</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A54" s="0">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D54" t="s" s="0">
         <v>9</v>
@@ -2542,9 +2542,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55" s="0">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C55" t="str" s="0">
         <f>Helper!D31</f>
@@ -2555,9 +2555,9 @@
         <v>Giant Water Bug</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A56" s="0">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F56" t="s" s="0">
         <v>11</v>
@@ -2566,9 +2566,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57" s="0">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C57" t="str" s="0">
         <f>Helper!D24</f>
@@ -2579,9 +2579,9 @@
         <v>Greater Flamingo</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A58" s="0">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D58" t="s" s="0">
         <v>10</v>
@@ -2590,9 +2590,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59" s="0">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C59" t="str" s="0">
         <f>Helper!D27</f>
@@ -2603,9 +2603,9 @@
         <v>Dyak Fruit Bat</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A60" s="0">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E60" t="s" s="0">
         <v>11</v>
@@ -2614,9 +2614,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A61" s="0">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C61" t="str" s="0">
         <f>Helper!D19</f>
@@ -2627,9 +2627,9 @@
         <v>Greater Rhea</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A62" s="0">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D62" t="s" s="0">
         <v>11</v>
@@ -2638,9 +2638,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A63" s="0">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C63" t="str" s="0">
         <f>Helper!D32</f>
@@ -2663,17 +2663,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97DD84F6-D856-4FCA-9254-65D9DBB06268}">
   <dimension ref="A1:O63"/>
   <sheetViews>
-    <sheetView zoomScale="56" zoomScaleNormal="39" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView tabSelected="1" topLeftCell="D38" zoomScale="56" zoomScaleNormal="39" workbookViewId="0">
+      <selection activeCell="N61" sqref="N61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="14.7109375"/>
-    <col min="3" max="15" customWidth="true" width="23.7109375"/>
+    <col min="2" max="2" customWidth="true" width="14.6640625"/>
+    <col min="3" max="15" customWidth="true" width="23.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="0">
         <v>0</v>
       </c>
@@ -2686,18 +2686,18 @@
         <v>Golden Eagle</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="0">
         <v>1</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>16</v>
+        <v>76</v>
       </c>
       <c r="N2" t="s" s="0">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="0">
         <v>2</v>
       </c>
@@ -2710,18 +2710,18 @@
         <v>Spongilla Fly</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="0">
         <v>3</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="M4" t="s" s="0">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="0">
         <v>4</v>
       </c>
@@ -2734,18 +2734,18 @@
         <v>Veined Octopus</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="0">
         <v>5</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="N6" t="s" s="0">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="0">
         <v>6</v>
       </c>
@@ -2758,18 +2758,18 @@
         <v>Puffer Fish</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="0">
         <v>7</v>
       </c>
       <c r="F8" t="s" s="0">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="L8" t="s" s="0">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="0">
         <v>8</v>
       </c>
@@ -2782,18 +2782,18 @@
         <v>Palaeocastor</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="0">
         <v>9</v>
       </c>
       <c r="D10" t="s" s="0">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="N10" t="s" s="0">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="0">
         <v>10</v>
       </c>
@@ -2806,18 +2806,18 @@
         <v>Trapdoor Spider</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="0">
         <v>11</v>
       </c>
       <c r="E12" t="s" s="0">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="M12" t="s" s="0">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="0">
         <v>12</v>
       </c>
@@ -2830,18 +2830,18 @@
         <v>Lungfish</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="0">
         <v>13</v>
       </c>
       <c r="D14" t="s" s="0">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="N14" t="s" s="0">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="0">
         <v>14</v>
       </c>
@@ -2854,18 +2854,18 @@
         <v>Tent-making Bat</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="0">
         <v>15</v>
       </c>
       <c r="G16" t="s" s="0">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="K16" t="s" s="0">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="0">
         <v>16</v>
       </c>
@@ -2878,18 +2878,18 @@
         <v>Goanna</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="0">
         <v>17</v>
       </c>
       <c r="D18" t="s" s="0">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="N18" t="s" s="0">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="0">
         <v>18</v>
       </c>
@@ -2902,18 +2902,18 @@
         <v>Rufous Hornero</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="0">
         <v>19</v>
       </c>
       <c r="E20" t="s" s="0">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="M20" t="s" s="0">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="0">
         <v>20</v>
       </c>
@@ -2926,18 +2926,18 @@
         <v>Homo habilis</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="0">
         <v>21</v>
       </c>
       <c r="D22" t="s" s="0">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="N22" t="s" s="0">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="0">
         <v>22</v>
       </c>
@@ -2950,18 +2950,18 @@
         <v>Bee</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="0">
         <v>23</v>
       </c>
       <c r="F24" t="s" s="0">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="L24" t="s" s="0">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="0">
         <v>24</v>
       </c>
@@ -2974,18 +2974,18 @@
         <v>Montezuma Oropendola</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="0">
         <v>25</v>
       </c>
       <c r="D26" t="s" s="0">
-        <v>27</v>
+        <v>71</v>
       </c>
       <c r="N26" t="s" s="0">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="0">
         <v>26</v>
       </c>
@@ -2998,18 +2998,18 @@
         <v>New Caledonian Crow</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="0">
         <v>27</v>
       </c>
       <c r="E28" t="s" s="0">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="M28" t="s" s="0">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="0">
         <v>28</v>
       </c>
@@ -3022,18 +3022,18 @@
         <v>Cathedral Termite</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="0">
         <v>29</v>
       </c>
       <c r="D30" t="s" s="0">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="N30" t="s" s="0">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" s="0">
         <v>30</v>
       </c>
@@ -3046,21 +3046,21 @@
         <v>Dung Beetle</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="0">
         <v>31</v>
       </c>
       <c r="H32" t="s" s="0">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="I32" t="s" s="0">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="J32" t="s" s="0">
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" s="0">
         <v>32</v>
       </c>
@@ -3073,7 +3073,7 @@
         <v>Emperor Penguin</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" s="0">
         <v>33</v>
       </c>
@@ -3082,25 +3082,25 @@
         <v>Bumblebee Bat</v>
       </c>
       <c r="D34" t="s" s="0">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="N34" t="s" s="0">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" s="0">
         <v>34</v>
       </c>
       <c r="C35" t="s" s="0">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="O35" t="str" s="0">
         <f>Helper!D66</f>
         <v>Lined Seahorse</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" s="0">
         <v>35</v>
       </c>
@@ -3109,13 +3109,13 @@
         <v>Shrew Mole</v>
       </c>
       <c r="E36" t="s" s="0">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="M36" t="s" s="0">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" s="0">
         <v>36</v>
       </c>
@@ -3128,18 +3128,18 @@
         <v>Owl Monkey</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" s="0">
         <v>37</v>
       </c>
       <c r="D38" t="s" s="0">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="N38" t="s" s="0">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" s="0">
         <v>38</v>
       </c>
@@ -3152,18 +3152,18 @@
         <v>Caspian Terns</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40" s="0">
         <v>39</v>
       </c>
       <c r="F40" t="s" s="0">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="L40" t="s" s="0">
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" s="0">
         <v>40</v>
       </c>
@@ -3176,18 +3176,18 @@
         <v>Pacific Spiny Lumpsucker</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" s="0">
         <v>41</v>
       </c>
       <c r="D42" t="s" s="0">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="N42" t="s" s="0">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" s="0">
         <v>42</v>
       </c>
@@ -3200,18 +3200,18 @@
         <v>Peacock Wrasse</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" s="0">
         <v>43</v>
       </c>
       <c r="E44" t="s" s="0">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="M44" t="s" s="0">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45" s="0">
         <v>44</v>
       </c>
@@ -3224,18 +3224,18 @@
         <v>Siamang</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46" s="0">
         <v>45</v>
       </c>
       <c r="D46" t="s" s="0">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="N46" t="s" s="0">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" s="0">
         <v>46</v>
       </c>
@@ -3248,18 +3248,18 @@
         <v>Darwin's Frogs</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" s="0">
         <v>47</v>
       </c>
       <c r="G48" t="s" s="0">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="K48" t="s" s="0">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" s="0">
         <v>48</v>
       </c>
@@ -3272,18 +3272,18 @@
         <v>Bat-Eared Fox</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50" s="0">
         <v>49</v>
       </c>
       <c r="D50" t="s" s="0">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="N50" t="s" s="0">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51" s="0">
         <v>50</v>
       </c>
@@ -3296,18 +3296,18 @@
         <v>Spotted sandpiper</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52" s="0">
         <v>51</v>
       </c>
       <c r="E52" t="s" s="0">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="M52" t="s" s="0">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A53" s="0">
         <v>52</v>
       </c>
@@ -3320,18 +3320,18 @@
         <v>Wolverine</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A54" s="0">
         <v>53</v>
       </c>
       <c r="D54" t="s" s="0">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="N54" t="s" s="0">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55" s="0">
         <v>54</v>
       </c>
@@ -3344,18 +3344,18 @@
         <v>Giant Water Bug</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A56" s="0">
         <v>55</v>
       </c>
       <c r="F56" t="s" s="0">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="L56" t="s" s="0">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57" s="0">
         <v>56</v>
       </c>
@@ -3368,18 +3368,18 @@
         <v>Greater Flamingo</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A58" s="0">
         <v>57</v>
       </c>
       <c r="D58" t="s" s="0">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="N58" t="s" s="0">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59" s="0">
         <v>58</v>
       </c>
@@ -3392,18 +3392,18 @@
         <v>Dyak Fruit Bat</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A60" s="0">
         <v>59</v>
       </c>
       <c r="E60" t="s" s="0">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="M60" t="s" s="0">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A61" s="0">
         <v>60</v>
       </c>
@@ -3416,18 +3416,18 @@
         <v>Greater Rhea</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A62" s="0">
         <v>61</v>
       </c>
       <c r="D62" t="s" s="0">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="N62" t="s" s="0">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A63" s="0">
         <v>62</v>
       </c>

</xml_diff>

<commit_message>
IDEK, ProgressGUI.java won't pull up the frame correctly when I pull it from Runner.java
</commit_message>
<xml_diff>
--- a/Resources/Bracket.xlsx
+++ b/Resources/Bracket.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1718" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1870" uniqueCount="81">
   <si>
     <t>Type in the two Wildcard animals below</t>
   </si>
@@ -2811,10 +2811,10 @@
         <v>11</v>
       </c>
       <c r="E12" t="s" s="0">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="M12" t="s" s="0">
-        <v>70</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
@@ -2835,10 +2835,10 @@
         <v>13</v>
       </c>
       <c r="D14" t="s" s="0">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="N14" t="s" s="0">
-        <v>31</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
@@ -2859,10 +2859,10 @@
         <v>15</v>
       </c>
       <c r="G16" t="s" s="0">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="K16" t="s" s="0">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
@@ -2907,10 +2907,10 @@
         <v>19</v>
       </c>
       <c r="E20" t="s" s="0">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="M20" t="s" s="0">
-        <v>72</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
@@ -2955,10 +2955,10 @@
         <v>23</v>
       </c>
       <c r="F24" t="s" s="0">
-        <v>35</v>
+        <v>71</v>
       </c>
       <c r="L24" t="s" s="0">
-        <v>79</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
@@ -2979,7 +2979,7 @@
         <v>25</v>
       </c>
       <c r="D26" t="s" s="0">
-        <v>25</v>
+        <v>71</v>
       </c>
       <c r="N26" t="s" s="0">
         <v>56</v>
@@ -3003,10 +3003,10 @@
         <v>27</v>
       </c>
       <c r="E28" t="s" s="0">
-        <v>35</v>
+        <v>71</v>
       </c>
       <c r="M28" t="s" s="0">
-        <v>79</v>
+        <v>21</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
@@ -3027,7 +3027,7 @@
         <v>29</v>
       </c>
       <c r="D30" t="s" s="0">
-        <v>35</v>
+        <v>78</v>
       </c>
       <c r="N30" t="s" s="0">
         <v>21</v>
@@ -3082,7 +3082,7 @@
         <v>Bumblebee Bat</v>
       </c>
       <c r="D34" t="s" s="0">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="N34" t="s" s="0">
         <v>22</v>
@@ -3157,7 +3157,7 @@
         <v>39</v>
       </c>
       <c r="F40" t="s" s="0">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="L40" t="s" s="0">
         <v>22</v>
@@ -3181,7 +3181,7 @@
         <v>41</v>
       </c>
       <c r="D42" t="s" s="0">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="N42" t="s" s="0">
         <v>45</v>
@@ -3205,10 +3205,10 @@
         <v>43</v>
       </c>
       <c r="E44" t="s" s="0">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="M44" t="s" s="0">
-        <v>58</v>
+        <v>24</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.3">
@@ -3229,10 +3229,10 @@
         <v>45</v>
       </c>
       <c r="D46" t="s" s="0">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="N46" t="s" s="0">
-        <v>59</v>
+        <v>24</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.3">
@@ -3277,7 +3277,7 @@
         <v>49</v>
       </c>
       <c r="D50" t="s" s="0">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="N50" t="s" s="0">
         <v>60</v>
@@ -3301,7 +3301,7 @@
         <v>51</v>
       </c>
       <c r="E52" t="s" s="0">
-        <v>33</v>
+        <v>77</v>
       </c>
       <c r="M52" t="s" s="0">
         <v>28</v>
@@ -3352,7 +3352,7 @@
         <v>18</v>
       </c>
       <c r="L56" t="s" s="0">
-        <v>61</v>
+        <v>26</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.3">
@@ -3373,7 +3373,7 @@
         <v>57</v>
       </c>
       <c r="D58" t="s" s="0">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="N58" t="s" s="0">
         <v>74</v>
@@ -3400,7 +3400,7 @@
         <v>18</v>
       </c>
       <c r="M60" t="s" s="0">
-        <v>61</v>
+        <v>26</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.3">
@@ -3421,7 +3421,7 @@
         <v>61</v>
       </c>
       <c r="D62" t="s" s="0">
-        <v>69</v>
+        <v>18</v>
       </c>
       <c r="N62" t="s" s="0">
         <v>26</v>

</xml_diff>

<commit_message>
tried fixing the problem, still doesn't work
</commit_message>
<xml_diff>
--- a/Resources/Bracket.xlsx
+++ b/Resources/Bracket.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1870" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1892" uniqueCount="81">
   <si>
     <t>Type in the two Wildcard animals below</t>
   </si>
@@ -2931,7 +2931,7 @@
         <v>21</v>
       </c>
       <c r="D22" t="s" s="0">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="N22" t="s" s="0">
         <v>20</v>
@@ -2979,7 +2979,7 @@
         <v>25</v>
       </c>
       <c r="D26" t="s" s="0">
-        <v>71</v>
+        <v>25</v>
       </c>
       <c r="N26" t="s" s="0">
         <v>56</v>
@@ -3082,7 +3082,7 @@
         <v>Bumblebee Bat</v>
       </c>
       <c r="D34" t="s" s="0">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="N34" t="s" s="0">
         <v>22</v>

</xml_diff>

<commit_message>
IDEK, still doesn't work
</commit_message>
<xml_diff>
--- a/Resources/Bracket.xlsx
+++ b/Resources/Bracket.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1892" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1956" uniqueCount="81">
   <si>
     <t>Type in the two Wildcard animals below</t>
   </si>
@@ -2715,7 +2715,7 @@
         <v>3</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="M4" t="s" s="0">
         <v>19</v>
@@ -2763,7 +2763,7 @@
         <v>7</v>
       </c>
       <c r="F8" t="s" s="0">
-        <v>16</v>
+        <v>68</v>
       </c>
       <c r="L8" t="s" s="0">
         <v>19</v>
@@ -2787,10 +2787,10 @@
         <v>9</v>
       </c>
       <c r="D10" t="s" s="0">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="N10" t="s" s="0">
-        <v>41</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
@@ -2814,7 +2814,7 @@
         <v>68</v>
       </c>
       <c r="M12" t="s" s="0">
-        <v>41</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
@@ -2838,7 +2838,7 @@
         <v>68</v>
       </c>
       <c r="N14" t="s" s="0">
-        <v>70</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
@@ -2859,10 +2859,10 @@
         <v>15</v>
       </c>
       <c r="G16" t="s" s="0">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="K16" t="s" s="0">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
@@ -2886,7 +2886,7 @@
         <v>42</v>
       </c>
       <c r="N18" t="s" s="0">
-        <v>43</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
@@ -2907,10 +2907,10 @@
         <v>19</v>
       </c>
       <c r="E20" t="s" s="0">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="M20" t="s" s="0">
-        <v>20</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
@@ -2934,7 +2934,7 @@
         <v>17</v>
       </c>
       <c r="N22" t="s" s="0">
-        <v>20</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
@@ -2955,10 +2955,10 @@
         <v>23</v>
       </c>
       <c r="F24" t="s" s="0">
-        <v>71</v>
+        <v>35</v>
       </c>
       <c r="L24" t="s" s="0">
-        <v>21</v>
+        <v>79</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
@@ -2979,7 +2979,7 @@
         <v>25</v>
       </c>
       <c r="D26" t="s" s="0">
-        <v>25</v>
+        <v>71</v>
       </c>
       <c r="N26" t="s" s="0">
         <v>56</v>
@@ -3003,10 +3003,10 @@
         <v>27</v>
       </c>
       <c r="E28" t="s" s="0">
-        <v>71</v>
+        <v>35</v>
       </c>
       <c r="M28" t="s" s="0">
-        <v>21</v>
+        <v>79</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
@@ -3027,10 +3027,10 @@
         <v>29</v>
       </c>
       <c r="D30" t="s" s="0">
-        <v>78</v>
+        <v>35</v>
       </c>
       <c r="N30" t="s" s="0">
-        <v>21</v>
+        <v>79</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
@@ -3054,10 +3054,10 @@
         <v>18</v>
       </c>
       <c r="I32" t="s" s="0">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="J32" t="s" s="0">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.3">
@@ -3082,7 +3082,7 @@
         <v>Bumblebee Bat</v>
       </c>
       <c r="D34" t="s" s="0">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="N34" t="s" s="0">
         <v>22</v>
@@ -3112,7 +3112,7 @@
         <v>30</v>
       </c>
       <c r="M36" t="s" s="0">
-        <v>22</v>
+        <v>57</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.3">
@@ -3160,7 +3160,7 @@
         <v>30</v>
       </c>
       <c r="L40" t="s" s="0">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.3">
@@ -3181,10 +3181,10 @@
         <v>41</v>
       </c>
       <c r="D42" t="s" s="0">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="N42" t="s" s="0">
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.3">
@@ -3256,7 +3256,7 @@
         <v>18</v>
       </c>
       <c r="K48" t="s" s="0">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.3">
@@ -3301,10 +3301,10 @@
         <v>51</v>
       </c>
       <c r="E52" t="s" s="0">
-        <v>77</v>
+        <v>27</v>
       </c>
       <c r="M52" t="s" s="0">
-        <v>28</v>
+        <v>60</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.3">
@@ -3325,10 +3325,10 @@
         <v>53</v>
       </c>
       <c r="D54" t="s" s="0">
-        <v>77</v>
+        <v>27</v>
       </c>
       <c r="N54" t="s" s="0">
-        <v>28</v>
+        <v>75</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.3">
@@ -3373,10 +3373,10 @@
         <v>57</v>
       </c>
       <c r="D58" t="s" s="0">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="N58" t="s" s="0">
-        <v>74</v>
+        <v>29</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
added tool tip to progress bar
</commit_message>
<xml_diff>
--- a/Resources/Bracket.xlsx
+++ b/Resources/Bracket.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3293" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3546" uniqueCount="81">
   <si>
     <t>Type in the two Wildcard animals below</t>
   </si>
@@ -2691,7 +2691,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>76</v>
+        <v>16</v>
       </c>
       <c r="N2" t="s" s="0">
         <v>19</v>
@@ -2715,10 +2715,10 @@
         <v>3</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="M4" t="s" s="0">
-        <v>19</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -2763,7 +2763,7 @@
         <v>7</v>
       </c>
       <c r="F8" t="s" s="0">
-        <v>68</v>
+        <v>16</v>
       </c>
       <c r="L8" t="s" s="0">
         <v>19</v>
@@ -2790,7 +2790,7 @@
         <v>47</v>
       </c>
       <c r="N10" t="s" s="0">
-        <v>41</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
@@ -2811,10 +2811,10 @@
         <v>11</v>
       </c>
       <c r="E12" t="s" s="0">
-        <v>68</v>
+        <v>34</v>
       </c>
       <c r="M12" t="s" s="0">
-        <v>70</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
@@ -2835,10 +2835,10 @@
         <v>13</v>
       </c>
       <c r="D14" t="s" s="0">
-        <v>68</v>
+        <v>34</v>
       </c>
       <c r="N14" t="s" s="0">
-        <v>70</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
@@ -2859,7 +2859,7 @@
         <v>15</v>
       </c>
       <c r="G16" t="s" s="0">
-        <v>35</v>
+        <v>78</v>
       </c>
       <c r="K16" t="s" s="0">
         <v>21</v>
@@ -2955,7 +2955,7 @@
         <v>23</v>
       </c>
       <c r="F24" t="s" s="0">
-        <v>35</v>
+        <v>78</v>
       </c>
       <c r="L24" t="s" s="0">
         <v>21</v>
@@ -3051,7 +3051,7 @@
         <v>31</v>
       </c>
       <c r="H32" t="s" s="0">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="I32" t="s" s="0">
         <v>26</v>
@@ -3112,7 +3112,7 @@
         <v>30</v>
       </c>
       <c r="M36" t="s" s="0">
-        <v>57</v>
+        <v>22</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.3">
@@ -3184,7 +3184,7 @@
         <v>48</v>
       </c>
       <c r="N42" t="s" s="0">
-        <v>58</v>
+        <v>45</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.3">
@@ -3205,7 +3205,7 @@
         <v>43</v>
       </c>
       <c r="E44" t="s" s="0">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="M44" t="s" s="0">
         <v>24</v>
@@ -3229,7 +3229,7 @@
         <v>45</v>
       </c>
       <c r="D46" t="s" s="0">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="N46" t="s" s="0">
         <v>24</v>
@@ -3253,7 +3253,7 @@
         <v>47</v>
       </c>
       <c r="G48" t="s" s="0">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="K48" t="s" s="0">
         <v>26</v>
@@ -3277,10 +3277,10 @@
         <v>49</v>
       </c>
       <c r="D50" t="s" s="0">
-        <v>63</v>
+        <v>33</v>
       </c>
       <c r="N50" t="s" s="0">
-        <v>37</v>
+        <v>60</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.3">
@@ -3301,10 +3301,10 @@
         <v>51</v>
       </c>
       <c r="E52" t="s" s="0">
-        <v>77</v>
+        <v>27</v>
       </c>
       <c r="M52" t="s" s="0">
-        <v>28</v>
+        <v>75</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.3">
@@ -3325,10 +3325,10 @@
         <v>53</v>
       </c>
       <c r="D54" t="s" s="0">
-        <v>77</v>
+        <v>27</v>
       </c>
       <c r="N54" t="s" s="0">
-        <v>28</v>
+        <v>75</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.3">
@@ -3349,7 +3349,7 @@
         <v>55</v>
       </c>
       <c r="F56" t="s" s="0">
-        <v>69</v>
+        <v>18</v>
       </c>
       <c r="L56" t="s" s="0">
         <v>26</v>
@@ -3397,7 +3397,7 @@
         <v>59</v>
       </c>
       <c r="E60" t="s" s="0">
-        <v>69</v>
+        <v>18</v>
       </c>
       <c r="M60" t="s" s="0">
         <v>26</v>
@@ -3421,10 +3421,10 @@
         <v>61</v>
       </c>
       <c r="D62" t="s" s="0">
-        <v>69</v>
+        <v>18</v>
       </c>
       <c r="N62" t="s" s="0">
-        <v>26</v>
+        <v>61</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
idk, add times to progressBar ToolTipText
</commit_message>
<xml_diff>
--- a/Resources/Bracket.xlsx
+++ b/Resources/Bracket.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4347" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5564" uniqueCount="81">
   <si>
     <t>Type in the two Wildcard animals below</t>
   </si>
@@ -2718,7 +2718,7 @@
         <v>16</v>
       </c>
       <c r="M4" t="s" s="0">
-        <v>55</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -2763,7 +2763,7 @@
         <v>7</v>
       </c>
       <c r="F8" t="s" s="0">
-        <v>68</v>
+        <v>16</v>
       </c>
       <c r="L8" t="s" s="0">
         <v>31</v>
@@ -2811,7 +2811,7 @@
         <v>11</v>
       </c>
       <c r="E12" t="s" s="0">
-        <v>68</v>
+        <v>34</v>
       </c>
       <c r="M12" t="s" s="0">
         <v>31</v>
@@ -2835,7 +2835,7 @@
         <v>13</v>
       </c>
       <c r="D14" t="s" s="0">
-        <v>68</v>
+        <v>34</v>
       </c>
       <c r="N14" t="s" s="0">
         <v>31</v>
@@ -2859,7 +2859,7 @@
         <v>15</v>
       </c>
       <c r="G16" t="s" s="0">
-        <v>68</v>
+        <v>16</v>
       </c>
       <c r="K16" t="s" s="0">
         <v>21</v>
@@ -2886,7 +2886,7 @@
         <v>42</v>
       </c>
       <c r="N18" t="s" s="0">
-        <v>43</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
@@ -2910,7 +2910,7 @@
         <v>52</v>
       </c>
       <c r="M20" t="s" s="0">
-        <v>72</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
@@ -2934,7 +2934,7 @@
         <v>52</v>
       </c>
       <c r="N22" t="s" s="0">
-        <v>72</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
@@ -2955,7 +2955,7 @@
         <v>23</v>
       </c>
       <c r="F24" t="s" s="0">
-        <v>78</v>
+        <v>35</v>
       </c>
       <c r="L24" t="s" s="0">
         <v>21</v>
@@ -2979,7 +2979,7 @@
         <v>25</v>
       </c>
       <c r="D26" t="s" s="0">
-        <v>71</v>
+        <v>25</v>
       </c>
       <c r="N26" t="s" s="0">
         <v>56</v>
@@ -3003,7 +3003,7 @@
         <v>27</v>
       </c>
       <c r="E28" t="s" s="0">
-        <v>78</v>
+        <v>35</v>
       </c>
       <c r="M28" t="s" s="0">
         <v>21</v>
@@ -3027,7 +3027,7 @@
         <v>29</v>
       </c>
       <c r="D30" t="s" s="0">
-        <v>78</v>
+        <v>35</v>
       </c>
       <c r="N30" t="s" s="0">
         <v>21</v>
@@ -3109,7 +3109,7 @@
         <v>Shrew Mole</v>
       </c>
       <c r="E36" t="s" s="0">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="M36" t="s" s="0">
         <v>22</v>
@@ -3157,10 +3157,10 @@
         <v>39</v>
       </c>
       <c r="F40" t="s" s="0">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="L40" t="s" s="0">
-        <v>22</v>
+        <v>58</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.3">
@@ -3184,7 +3184,7 @@
         <v>48</v>
       </c>
       <c r="N42" t="s" s="0">
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.3">
@@ -3205,10 +3205,10 @@
         <v>43</v>
       </c>
       <c r="E44" t="s" s="0">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="M44" t="s" s="0">
-        <v>24</v>
+        <v>58</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.3">
@@ -3229,10 +3229,10 @@
         <v>45</v>
       </c>
       <c r="D46" t="s" s="0">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="N46" t="s" s="0">
-        <v>24</v>
+        <v>59</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.3">
@@ -3277,10 +3277,10 @@
         <v>49</v>
       </c>
       <c r="D50" t="s" s="0">
-        <v>63</v>
+        <v>33</v>
       </c>
       <c r="N50" t="s" s="0">
-        <v>60</v>
+        <v>37</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
IDK, toolTipText for the progress bar is working fine. Trying to make the program delete the last file it was working on, but I can't get it to work.
</commit_message>
<xml_diff>
--- a/Resources/Bracket.xlsx
+++ b/Resources/Bracket.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5919" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8497" uniqueCount="81">
   <si>
     <t>Type in the two Wildcard animals below</t>
   </si>
@@ -2691,7 +2691,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>16</v>
+        <v>76</v>
       </c>
       <c r="N2" t="s" s="0">
         <v>80</v>
@@ -2715,7 +2715,7 @@
         <v>3</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="M4" t="s" s="0">
         <v>19</v>
@@ -2763,10 +2763,10 @@
         <v>7</v>
       </c>
       <c r="F8" t="s" s="0">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="L8" t="s" s="0">
-        <v>31</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
@@ -2787,7 +2787,7 @@
         <v>9</v>
       </c>
       <c r="D10" t="s" s="0">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="N10" t="s" s="0">
         <v>65</v>
@@ -2814,7 +2814,7 @@
         <v>34</v>
       </c>
       <c r="M12" t="s" s="0">
-        <v>31</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
@@ -2835,10 +2835,10 @@
         <v>13</v>
       </c>
       <c r="D14" t="s" s="0">
-        <v>68</v>
+        <v>34</v>
       </c>
       <c r="N14" t="s" s="0">
-        <v>31</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
@@ -2859,7 +2859,7 @@
         <v>15</v>
       </c>
       <c r="G16" t="s" s="0">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="K16" t="s" s="0">
         <v>21</v>
@@ -2907,7 +2907,7 @@
         <v>19</v>
       </c>
       <c r="E20" t="s" s="0">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="M20" t="s" s="0">
         <v>20</v>
@@ -2934,7 +2934,7 @@
         <v>17</v>
       </c>
       <c r="N22" t="s" s="0">
-        <v>72</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
@@ -2955,7 +2955,7 @@
         <v>23</v>
       </c>
       <c r="F24" t="s" s="0">
-        <v>78</v>
+        <v>35</v>
       </c>
       <c r="L24" t="s" s="0">
         <v>21</v>
@@ -2982,7 +2982,7 @@
         <v>71</v>
       </c>
       <c r="N26" t="s" s="0">
-        <v>56</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
@@ -3051,10 +3051,10 @@
         <v>31</v>
       </c>
       <c r="H32" t="s" s="0">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="I32" t="s" s="0">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="J32" t="s" s="0">
         <v>26</v>
@@ -3082,7 +3082,7 @@
         <v>Bumblebee Bat</v>
       </c>
       <c r="D34" t="s" s="0">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="N34" t="s" s="0">
         <v>22</v>
@@ -3112,7 +3112,7 @@
         <v>53</v>
       </c>
       <c r="M36" t="s" s="0">
-        <v>22</v>
+        <v>57</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.3">
@@ -3157,10 +3157,10 @@
         <v>39</v>
       </c>
       <c r="F40" t="s" s="0">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="L40" t="s" s="0">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.3">
@@ -3181,7 +3181,7 @@
         <v>41</v>
       </c>
       <c r="D42" t="s" s="0">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="N42" t="s" s="0">
         <v>45</v>
@@ -3205,10 +3205,10 @@
         <v>43</v>
       </c>
       <c r="E44" t="s" s="0">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="M44" t="s" s="0">
-        <v>59</v>
+        <v>24</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.3">
@@ -3232,7 +3232,7 @@
         <v>62</v>
       </c>
       <c r="N46" t="s" s="0">
-        <v>59</v>
+        <v>24</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.3">
@@ -3253,7 +3253,7 @@
         <v>47</v>
       </c>
       <c r="G48" t="s" s="0">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="K48" t="s" s="0">
         <v>26</v>
@@ -3301,10 +3301,10 @@
         <v>51</v>
       </c>
       <c r="E52" t="s" s="0">
-        <v>77</v>
+        <v>27</v>
       </c>
       <c r="M52" t="s" s="0">
-        <v>28</v>
+        <v>75</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.3">
@@ -3325,10 +3325,10 @@
         <v>53</v>
       </c>
       <c r="D54" t="s" s="0">
-        <v>27</v>
+        <v>77</v>
       </c>
       <c r="N54" t="s" s="0">
-        <v>28</v>
+        <v>75</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.3">
@@ -3349,7 +3349,7 @@
         <v>55</v>
       </c>
       <c r="F56" t="s" s="0">
-        <v>69</v>
+        <v>18</v>
       </c>
       <c r="L56" t="s" s="0">
         <v>26</v>

</xml_diff>

<commit_message>
tried to start to download resources files in case the resource folder does not have the right resources needed.
</commit_message>
<xml_diff>
--- a/Resources/Bracket.xlsx
+++ b/Resources/Bracket.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10828" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10892" uniqueCount="81">
   <si>
     <t>Type in the two Wildcard animals below</t>
   </si>
@@ -2691,10 +2691,10 @@
         <v>1</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>16</v>
+        <v>76</v>
       </c>
       <c r="N2" t="s" s="0">
-        <v>19</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
@@ -2715,10 +2715,10 @@
         <v>3</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>16</v>
+        <v>76</v>
       </c>
       <c r="M4" t="s" s="0">
-        <v>19</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -2739,10 +2739,10 @@
         <v>5</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="N6" t="s" s="0">
-        <v>40</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
@@ -2763,10 +2763,10 @@
         <v>7</v>
       </c>
       <c r="F8" t="s" s="0">
-        <v>16</v>
+        <v>76</v>
       </c>
       <c r="L8" t="s" s="0">
-        <v>19</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
@@ -2787,10 +2787,10 @@
         <v>9</v>
       </c>
       <c r="D10" t="s" s="0">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="N10" t="s" s="0">
-        <v>41</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
@@ -2811,10 +2811,10 @@
         <v>11</v>
       </c>
       <c r="E12" t="s" s="0">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="M12" t="s" s="0">
-        <v>31</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
@@ -2835,10 +2835,10 @@
         <v>13</v>
       </c>
       <c r="D14" t="s" s="0">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="N14" t="s" s="0">
-        <v>31</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
@@ -2859,10 +2859,10 @@
         <v>15</v>
       </c>
       <c r="G16" t="s" s="0">
-        <v>16</v>
+        <v>76</v>
       </c>
       <c r="K16" t="s" s="0">
-        <v>19</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
@@ -2883,10 +2883,10 @@
         <v>17</v>
       </c>
       <c r="D18" t="s" s="0">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="N18" t="s" s="0">
-        <v>66</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
@@ -2907,10 +2907,10 @@
         <v>19</v>
       </c>
       <c r="E20" t="s" s="0">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="M20" t="s" s="0">
-        <v>20</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
@@ -2931,10 +2931,10 @@
         <v>21</v>
       </c>
       <c r="D22" t="s" s="0">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="N22" t="s" s="0">
-        <v>20</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
@@ -2955,10 +2955,10 @@
         <v>23</v>
       </c>
       <c r="F24" t="s" s="0">
-        <v>35</v>
+        <v>78</v>
       </c>
       <c r="L24" t="s" s="0">
-        <v>21</v>
+        <v>79</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
@@ -2979,10 +2979,10 @@
         <v>25</v>
       </c>
       <c r="D26" t="s" s="0">
-        <v>25</v>
+        <v>71</v>
       </c>
       <c r="N26" t="s" s="0">
-        <v>44</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
@@ -3003,10 +3003,10 @@
         <v>27</v>
       </c>
       <c r="E28" t="s" s="0">
-        <v>35</v>
+        <v>78</v>
       </c>
       <c r="M28" t="s" s="0">
-        <v>21</v>
+        <v>79</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
@@ -3027,10 +3027,10 @@
         <v>29</v>
       </c>
       <c r="D30" t="s" s="0">
-        <v>35</v>
+        <v>78</v>
       </c>
       <c r="N30" t="s" s="0">
-        <v>21</v>
+        <v>79</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
@@ -3051,13 +3051,13 @@
         <v>31</v>
       </c>
       <c r="H32" t="s" s="0">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="I32" t="s" s="0">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="J32" t="s" s="0">
-        <v>19</v>
+        <v>80</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.3">
@@ -3082,10 +3082,10 @@
         <v>Bumblebee Bat</v>
       </c>
       <c r="D34" t="s" s="0">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="N34" t="s" s="0">
-        <v>22</v>
+        <v>73</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.3">
@@ -3093,7 +3093,7 @@
         <v>34</v>
       </c>
       <c r="C35" t="s" s="0">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="O35" t="str" s="0">
         <f>Helper!D66</f>
@@ -3109,10 +3109,10 @@
         <v>Shrew Mole</v>
       </c>
       <c r="E36" t="s" s="0">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="M36" t="s" s="0">
-        <v>22</v>
+        <v>73</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.3">
@@ -3133,10 +3133,10 @@
         <v>37</v>
       </c>
       <c r="D38" t="s" s="0">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="N38" t="s" s="0">
-        <v>23</v>
+        <v>57</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.3">
@@ -3157,10 +3157,10 @@
         <v>39</v>
       </c>
       <c r="F40" t="s" s="0">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="L40" t="s" s="0">
-        <v>22</v>
+        <v>73</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.3">
@@ -3181,10 +3181,10 @@
         <v>41</v>
       </c>
       <c r="D42" t="s" s="0">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="N42" t="s" s="0">
-        <v>58</v>
+        <v>45</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.3">
@@ -3205,10 +3205,10 @@
         <v>43</v>
       </c>
       <c r="E44" t="s" s="0">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="M44" t="s" s="0">
-        <v>24</v>
+        <v>59</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.3">
@@ -3229,10 +3229,10 @@
         <v>45</v>
       </c>
       <c r="D46" t="s" s="0">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="N46" t="s" s="0">
-        <v>24</v>
+        <v>59</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.3">
@@ -3253,10 +3253,10 @@
         <v>47</v>
       </c>
       <c r="G48" t="s" s="0">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="K48" t="s" s="0">
-        <v>22</v>
+        <v>73</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.3">
@@ -3277,10 +3277,10 @@
         <v>49</v>
       </c>
       <c r="D50" t="s" s="0">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="N50" t="s" s="0">
-        <v>37</v>
+        <v>60</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.3">
@@ -3301,10 +3301,10 @@
         <v>51</v>
       </c>
       <c r="E52" t="s" s="0">
-        <v>27</v>
+        <v>77</v>
       </c>
       <c r="M52" t="s" s="0">
-        <v>28</v>
+        <v>75</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.3">
@@ -3325,10 +3325,10 @@
         <v>53</v>
       </c>
       <c r="D54" t="s" s="0">
-        <v>27</v>
+        <v>77</v>
       </c>
       <c r="N54" t="s" s="0">
-        <v>28</v>
+        <v>75</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.3">
@@ -3349,10 +3349,10 @@
         <v>55</v>
       </c>
       <c r="F56" t="s" s="0">
-        <v>18</v>
+        <v>69</v>
       </c>
       <c r="L56" t="s" s="0">
-        <v>26</v>
+        <v>61</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.3">
@@ -3373,10 +3373,10 @@
         <v>57</v>
       </c>
       <c r="D58" t="s" s="0">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="N58" t="s" s="0">
-        <v>29</v>
+        <v>74</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.3">
@@ -3397,10 +3397,10 @@
         <v>59</v>
       </c>
       <c r="E60" t="s" s="0">
-        <v>18</v>
+        <v>69</v>
       </c>
       <c r="M60" t="s" s="0">
-        <v>26</v>
+        <v>61</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.3">
@@ -3421,10 +3421,10 @@
         <v>61</v>
       </c>
       <c r="D62" t="s" s="0">
-        <v>18</v>
+        <v>69</v>
       </c>
       <c r="N62" t="s" s="0">
-        <v>26</v>
+        <v>61</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
make stuff private and non-static so the protection is better.
</commit_message>
<xml_diff>
--- a/Resources/Bracket.xlsx
+++ b/Resources/Bracket.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10892" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11277" uniqueCount="81">
   <si>
     <t>Type in the two Wildcard animals below</t>
   </si>
@@ -2691,10 +2691,10 @@
         <v>1</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>76</v>
+        <v>16</v>
       </c>
       <c r="N2" t="s" s="0">
-        <v>80</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
@@ -2715,10 +2715,10 @@
         <v>3</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>76</v>
+        <v>16</v>
       </c>
       <c r="M4" t="s" s="0">
-        <v>80</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -2739,10 +2739,10 @@
         <v>5</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="N6" t="s" s="0">
-        <v>55</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
@@ -2763,10 +2763,10 @@
         <v>7</v>
       </c>
       <c r="F8" t="s" s="0">
-        <v>76</v>
+        <v>16</v>
       </c>
       <c r="L8" t="s" s="0">
-        <v>80</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
@@ -2787,10 +2787,10 @@
         <v>9</v>
       </c>
       <c r="D10" t="s" s="0">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="N10" t="s" s="0">
-        <v>65</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
@@ -2811,10 +2811,10 @@
         <v>11</v>
       </c>
       <c r="E12" t="s" s="0">
-        <v>68</v>
+        <v>34</v>
       </c>
       <c r="M12" t="s" s="0">
-        <v>70</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
@@ -2835,10 +2835,10 @@
         <v>13</v>
       </c>
       <c r="D14" t="s" s="0">
-        <v>68</v>
+        <v>34</v>
       </c>
       <c r="N14" t="s" s="0">
-        <v>70</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
@@ -2859,10 +2859,10 @@
         <v>15</v>
       </c>
       <c r="G16" t="s" s="0">
-        <v>76</v>
+        <v>16</v>
       </c>
       <c r="K16" t="s" s="0">
-        <v>80</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
@@ -2883,10 +2883,10 @@
         <v>17</v>
       </c>
       <c r="D18" t="s" s="0">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="N18" t="s" s="0">
-        <v>43</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
@@ -2907,10 +2907,10 @@
         <v>19</v>
       </c>
       <c r="E20" t="s" s="0">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="M20" t="s" s="0">
-        <v>72</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
@@ -2931,10 +2931,10 @@
         <v>21</v>
       </c>
       <c r="D22" t="s" s="0">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="N22" t="s" s="0">
-        <v>72</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
@@ -2955,10 +2955,10 @@
         <v>23</v>
       </c>
       <c r="F24" t="s" s="0">
-        <v>78</v>
+        <v>35</v>
       </c>
       <c r="L24" t="s" s="0">
-        <v>79</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
@@ -2979,10 +2979,10 @@
         <v>25</v>
       </c>
       <c r="D26" t="s" s="0">
-        <v>71</v>
+        <v>25</v>
       </c>
       <c r="N26" t="s" s="0">
-        <v>56</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
@@ -3003,10 +3003,10 @@
         <v>27</v>
       </c>
       <c r="E28" t="s" s="0">
-        <v>78</v>
+        <v>35</v>
       </c>
       <c r="M28" t="s" s="0">
-        <v>79</v>
+        <v>21</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
@@ -3027,10 +3027,10 @@
         <v>29</v>
       </c>
       <c r="D30" t="s" s="0">
-        <v>78</v>
+        <v>35</v>
       </c>
       <c r="N30" t="s" s="0">
-        <v>79</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
@@ -3051,13 +3051,13 @@
         <v>31</v>
       </c>
       <c r="H32" t="s" s="0">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="I32" t="s" s="0">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="J32" t="s" s="0">
-        <v>80</v>
+        <v>19</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.3">
@@ -3082,10 +3082,10 @@
         <v>Bumblebee Bat</v>
       </c>
       <c r="D34" t="s" s="0">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="N34" t="s" s="0">
-        <v>73</v>
+        <v>22</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.3">
@@ -3109,10 +3109,10 @@
         <v>Shrew Mole</v>
       </c>
       <c r="E36" t="s" s="0">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="M36" t="s" s="0">
-        <v>73</v>
+        <v>22</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.3">
@@ -3133,10 +3133,10 @@
         <v>37</v>
       </c>
       <c r="D38" t="s" s="0">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="N38" t="s" s="0">
-        <v>57</v>
+        <v>23</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.3">
@@ -3157,10 +3157,10 @@
         <v>39</v>
       </c>
       <c r="F40" t="s" s="0">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="L40" t="s" s="0">
-        <v>73</v>
+        <v>22</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.3">
@@ -3181,10 +3181,10 @@
         <v>41</v>
       </c>
       <c r="D42" t="s" s="0">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="N42" t="s" s="0">
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.3">
@@ -3205,10 +3205,10 @@
         <v>43</v>
       </c>
       <c r="E44" t="s" s="0">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="M44" t="s" s="0">
-        <v>59</v>
+        <v>24</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.3">
@@ -3229,10 +3229,10 @@
         <v>45</v>
       </c>
       <c r="D46" t="s" s="0">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="N46" t="s" s="0">
-        <v>59</v>
+        <v>24</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.3">
@@ -3253,10 +3253,10 @@
         <v>47</v>
       </c>
       <c r="G48" t="s" s="0">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="K48" t="s" s="0">
-        <v>73</v>
+        <v>22</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.3">
@@ -3277,10 +3277,10 @@
         <v>49</v>
       </c>
       <c r="D50" t="s" s="0">
-        <v>63</v>
+        <v>33</v>
       </c>
       <c r="N50" t="s" s="0">
-        <v>60</v>
+        <v>37</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.3">
@@ -3301,10 +3301,10 @@
         <v>51</v>
       </c>
       <c r="E52" t="s" s="0">
-        <v>77</v>
+        <v>27</v>
       </c>
       <c r="M52" t="s" s="0">
-        <v>75</v>
+        <v>28</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.3">
@@ -3325,10 +3325,10 @@
         <v>53</v>
       </c>
       <c r="D54" t="s" s="0">
-        <v>77</v>
+        <v>27</v>
       </c>
       <c r="N54" t="s" s="0">
-        <v>75</v>
+        <v>28</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.3">
@@ -3349,10 +3349,10 @@
         <v>55</v>
       </c>
       <c r="F56" t="s" s="0">
-        <v>69</v>
+        <v>18</v>
       </c>
       <c r="L56" t="s" s="0">
-        <v>61</v>
+        <v>26</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.3">
@@ -3373,10 +3373,10 @@
         <v>57</v>
       </c>
       <c r="D58" t="s" s="0">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="N58" t="s" s="0">
-        <v>74</v>
+        <v>29</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.3">
@@ -3397,10 +3397,10 @@
         <v>59</v>
       </c>
       <c r="E60" t="s" s="0">
-        <v>69</v>
+        <v>18</v>
       </c>
       <c r="M60" t="s" s="0">
-        <v>61</v>
+        <v>26</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.3">
@@ -3421,10 +3421,10 @@
         <v>61</v>
       </c>
       <c r="D62" t="s" s="0">
-        <v>69</v>
+        <v>18</v>
       </c>
       <c r="N62" t="s" s="0">
-        <v>61</v>
+        <v>26</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Made changes for new animals and bracket.
Need to make bigger Text.
</commit_message>
<xml_diff>
--- a/Resources/Bracket.xlsx
+++ b/Resources/Bracket.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20406"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pants\IdeaProjects\Mam\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ks4292\InteliJ\Mam\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{814F9D21-F62F-4EEB-922D-8204F3C797E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FDC6BE4-283F-4AE3-84E9-838C266081F1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8928" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="17280" windowHeight="8925" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Helper" sheetId="2" r:id="rId1"/>
@@ -21,24 +21,11 @@
     <externalReference r:id="rId4"/>
   </externalReferences>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11853" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="96">
   <si>
     <t>Type in the two Wildcard animals below</t>
   </si>
@@ -109,15 +96,9 @@
     <t>Emperor Penguin</t>
   </si>
   <si>
-    <t>Owl Monkey</t>
-  </si>
-  <si>
     <t>Siamang</t>
   </si>
   <si>
-    <t>Striped Rabbit</t>
-  </si>
-  <si>
     <t>Greater Rhea</t>
   </si>
   <si>
@@ -139,54 +120,21 @@
     <t>Southern Ningaui</t>
   </si>
   <si>
-    <t>Itjaritjari</t>
-  </si>
-  <si>
     <t>Striped dolphin</t>
   </si>
   <si>
     <t>Kudu</t>
   </si>
   <si>
-    <t>Mara</t>
-  </si>
-  <si>
-    <t>Bat-Eared Fox</t>
-  </si>
-  <si>
     <t>Bulldog Bat</t>
   </si>
   <si>
-    <t>Shrew Mole</t>
-  </si>
-  <si>
-    <t>Veined Octopus</t>
-  </si>
-  <si>
     <t>Palaeocastor</t>
   </si>
   <si>
-    <t>Highland Streaked Tenrec</t>
-  </si>
-  <si>
-    <t>Rufous Hornero</t>
-  </si>
-  <si>
-    <t>Montezuma Oropendola</t>
-  </si>
-  <si>
-    <t>Peacock Wrasse</t>
-  </si>
-  <si>
     <t>Giant striped mongoose</t>
   </si>
   <si>
-    <t>Striped Possum</t>
-  </si>
-  <si>
-    <t>Silver Pika</t>
-  </si>
-  <si>
     <t>Bumblebee Bat</t>
   </si>
   <si>
@@ -196,12 +144,6 @@
     <t>Wildcat</t>
   </si>
   <si>
-    <t>Fire-footed Rope Squirrel</t>
-  </si>
-  <si>
-    <t>Grasshopper Mouse</t>
-  </si>
-  <si>
     <t>Sibree Dwarf Lemur</t>
   </si>
   <si>
@@ -217,70 +159,160 @@
     <t>Pacific Spiny Lumpsucker</t>
   </si>
   <si>
-    <t>Darwin's Frogs</t>
-  </si>
-  <si>
     <t>Spotted sandpiper</t>
   </si>
   <si>
-    <t xml:space="preserve">Three-Spined stickleback </t>
-  </si>
-  <si>
     <t>Siberian Chipmunk</t>
   </si>
   <si>
     <t>Silky Anteater</t>
   </si>
   <si>
-    <t>Thor's Hero Shrew</t>
-  </si>
-  <si>
-    <t>Trapdoor Spider</t>
-  </si>
-  <si>
     <t>Goanna</t>
   </si>
   <si>
-    <t>Striped Polecat</t>
-  </si>
-  <si>
-    <t>Chequered elephant shrew</t>
-  </si>
-  <si>
-    <t>Pygmy Jerboa</t>
-  </si>
-  <si>
-    <t>Tent-making Bat</t>
-  </si>
-  <si>
     <t>Numbat</t>
   </si>
   <si>
-    <t>Bee</t>
-  </si>
-  <si>
-    <t>Lined Seahorse</t>
-  </si>
-  <si>
-    <t>Dyak Fruit Bat</t>
-  </si>
-  <si>
-    <t>Giant Water Bug</t>
-  </si>
-  <si>
-    <t>Four-Striped Grass Mouse</t>
-  </si>
-  <si>
-    <t>Colo Colo Opossum</t>
-  </si>
-  <si>
-    <t>Badger Bat</t>
-  </si>
-  <si>
-    <t>Dung Beetle</t>
-  </si>
-  <si>
-    <t>Spongilla Fly</t>
+    <t>Rainbow Grasshopper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sperm Whale </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raven </t>
+  </si>
+  <si>
+    <t>Stag</t>
+  </si>
+  <si>
+    <t>Wolf</t>
+  </si>
+  <si>
+    <t>Indian Grey Mongoose</t>
+  </si>
+  <si>
+    <t>Catfish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lucy </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Giant Squid </t>
+  </si>
+  <si>
+    <t>Nicobar Pigeon</t>
+  </si>
+  <si>
+    <t>Halloween Crab</t>
+  </si>
+  <si>
+    <t>Marbled Polecat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peacock Mantis Shrimp </t>
+  </si>
+  <si>
+    <t>Wolf's Mona Monkey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Golden-headed Lion Tamarin </t>
+  </si>
+  <si>
+    <t>Red-shanked Douc</t>
+  </si>
+  <si>
+    <t>Kob</t>
+  </si>
+  <si>
+    <t>Hairy-legged Bee</t>
+  </si>
+  <si>
+    <t>Tufted Ground Squirrel</t>
+  </si>
+  <si>
+    <t>Koala</t>
+  </si>
+  <si>
+    <t>Fork-marked Lemur</t>
+  </si>
+  <si>
+    <t>Porcupine</t>
+  </si>
+  <si>
+    <t>Pitcher Plant</t>
+  </si>
+  <si>
+    <t>Parasitic Guest Ant</t>
+  </si>
+  <si>
+    <t>Northern Elephant Seal</t>
+  </si>
+  <si>
+    <t>Opossum</t>
+  </si>
+  <si>
+    <t>Pronghorn</t>
+  </si>
+  <si>
+    <t>Singing Mouse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Howler Monkey </t>
+  </si>
+  <si>
+    <t>Elegant Dancing Frog</t>
+  </si>
+  <si>
+    <t>Flame Bowerbird</t>
+  </si>
+  <si>
+    <t>Forest Elephant</t>
+  </si>
+  <si>
+    <t>Sparklemuffin Peacock Spider</t>
+  </si>
+  <si>
+    <t>Starling</t>
+  </si>
+  <si>
+    <t>Tiger</t>
+  </si>
+  <si>
+    <t>Painted Wild Dog</t>
+  </si>
+  <si>
+    <t>Himalayan Monal</t>
+  </si>
+  <si>
+    <t>Madagascan Sunset Moth</t>
+  </si>
+  <si>
+    <t>Mottled Cup Moth</t>
+  </si>
+  <si>
+    <t>Chestnut-headed Bee-eater</t>
+  </si>
+  <si>
+    <t>Cobra Lily</t>
+  </si>
+  <si>
+    <t>Velvet Worm</t>
+  </si>
+  <si>
+    <t>Northern Short-tailed Shrew</t>
+  </si>
+  <si>
+    <t>Wrinkle-faced Bat</t>
+  </si>
+  <si>
+    <t>Leatherback Turtle</t>
+  </si>
+  <si>
+    <t>Great White Shark</t>
+  </si>
+  <si>
+    <t>Coral Snake</t>
   </si>
 </sst>
 </file>
@@ -346,336 +378,336 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Sheet1"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
-        <row r="2">
-          <cell r="C2" t="str">
-            <v>Sea Otter</v>
-          </cell>
-        </row>
         <row r="3">
           <cell r="C3" t="str">
-            <v xml:space="preserve">Rock Hyrax </v>
+            <v xml:space="preserve">Sperm Whale </v>
           </cell>
         </row>
         <row r="4">
           <cell r="C4" t="str">
-            <v>Dik Dik</v>
+            <v xml:space="preserve">Giant Squid </v>
           </cell>
         </row>
         <row r="5">
           <cell r="C5" t="str">
-            <v>Mara</v>
+            <v>Tiger</v>
           </cell>
         </row>
         <row r="6">
           <cell r="C6" t="str">
-            <v>Sibree Dwarf Lemur</v>
+            <v>Wolf</v>
           </cell>
         </row>
         <row r="7">
           <cell r="C7" t="str">
-            <v>Itjaritjari</v>
+            <v>Stag</v>
           </cell>
         </row>
         <row r="8">
           <cell r="C8" t="str">
-            <v>Bulldog Bat</v>
+            <v>Boar</v>
           </cell>
         </row>
         <row r="9">
           <cell r="C9" t="str">
-            <v>Southern Ningaui</v>
+            <v xml:space="preserve">Lucy </v>
           </cell>
         </row>
         <row r="10">
           <cell r="C10" t="str">
-            <v>Grasshopper Mouse</v>
+            <v xml:space="preserve">Raven </v>
           </cell>
         </row>
         <row r="11">
           <cell r="C11" t="str">
-            <v>Thor's Hero Shrew</v>
+            <v>Wandering Albatross</v>
           </cell>
         </row>
         <row r="12">
           <cell r="C12" t="str">
-            <v>Silky Anteater</v>
+            <v>Bigeye Houndshark</v>
           </cell>
         </row>
         <row r="13">
           <cell r="C13" t="str">
-            <v>Silver Pika</v>
+            <v>Indian Grey Mongoose</v>
           </cell>
         </row>
         <row r="14">
           <cell r="C14" t="str">
-            <v>Siberian Chipmunk</v>
+            <v>Starling</v>
           </cell>
         </row>
         <row r="15">
           <cell r="C15" t="str">
-            <v>Colo Colo Opossum</v>
+            <v>Harvest Mouse</v>
           </cell>
         </row>
         <row r="16">
           <cell r="C16" t="str">
-            <v>Pygmy Jerboa</v>
+            <v>Catfish</v>
           </cell>
         </row>
         <row r="17">
           <cell r="C17" t="str">
-            <v>Bumblebee Bat</v>
+            <v>Tarzan Chameleon</v>
           </cell>
         </row>
         <row r="18">
           <cell r="C18" t="str">
-            <v>Shrew Mole</v>
+            <v>Schizomid</v>
           </cell>
         </row>
         <row r="19">
           <cell r="C19" t="str">
-            <v>Okapi</v>
+            <v>Painted Wild Dog</v>
           </cell>
         </row>
         <row r="20">
           <cell r="C20" t="str">
-            <v>Kudu</v>
+            <v>Red-shanked Douc</v>
           </cell>
         </row>
         <row r="21">
           <cell r="C21" t="str">
-            <v>Striped hyena</v>
+            <v>Wolf's Mona Monkey</v>
           </cell>
         </row>
         <row r="22">
           <cell r="C22" t="str">
-            <v>Striped dolphin</v>
+            <v>Marbled Polecat</v>
           </cell>
         </row>
         <row r="23">
           <cell r="C23" t="str">
-            <v>Side-striped jackal</v>
+            <v>Halloween Crab</v>
           </cell>
         </row>
         <row r="24">
           <cell r="C24" t="str">
-            <v>Wildcat</v>
+            <v xml:space="preserve">Peacock Mantis Shrimp </v>
           </cell>
         </row>
         <row r="25">
           <cell r="C25" t="str">
-            <v>Striped Rabbit</v>
+            <v xml:space="preserve">Golden-headed Lion Tamarin </v>
           </cell>
         </row>
         <row r="26">
           <cell r="C26" t="str">
-            <v>Striped Polecat</v>
+            <v>Himalayan Monal</v>
           </cell>
         </row>
         <row r="27">
           <cell r="C27" t="str">
-            <v>Giant striped mongoose</v>
+            <v>Nicobar Pigeon</v>
           </cell>
         </row>
         <row r="28">
           <cell r="C28" t="str">
-            <v>Numbat</v>
+            <v>Mottled Cup Moth</v>
           </cell>
         </row>
         <row r="29">
           <cell r="C29" t="str">
-            <v>Highland Streaked Tenrec</v>
+            <v>Mandarin Fish</v>
           </cell>
         </row>
         <row r="30">
           <cell r="C30" t="str">
-            <v>Striped Possum</v>
+            <v>Bornean Rainbow Toad</v>
           </cell>
         </row>
         <row r="31">
           <cell r="C31" t="str">
-            <v>Chequered elephant shrew</v>
+            <v>Madagascan Sunset Moth</v>
           </cell>
         </row>
         <row r="32">
           <cell r="C32" t="str">
-            <v>Fire-footed Rope Squirrel</v>
+            <v>Flat Lizard</v>
           </cell>
         </row>
         <row r="33">
           <cell r="C33" t="str">
-            <v>Badger Bat</v>
+            <v>Rainbow Scarab</v>
           </cell>
         </row>
         <row r="34">
           <cell r="C34" t="str">
-            <v>Four-Striped Grass Mouse</v>
+            <v>Sparklemuffin Peacock Spider</v>
           </cell>
         </row>
         <row r="35">
           <cell r="C35" t="str">
-            <v>Emperor Penguin</v>
+            <v>Rainbow Grasshopper</v>
           </cell>
         </row>
         <row r="36">
           <cell r="C36" t="str">
-            <v>Greater Rhea</v>
+            <v>Northern Elephant Seal</v>
           </cell>
         </row>
         <row r="37">
           <cell r="C37" t="str">
-            <v>Wolverine</v>
+            <v>Forest Elephant</v>
           </cell>
         </row>
         <row r="38">
           <cell r="C38" t="str">
-            <v>Siamang</v>
+            <v>Great White Shark</v>
           </cell>
         </row>
         <row r="39">
           <cell r="C39" t="str">
-            <v>Pacific Spiny Lumpsucker</v>
+            <v>Leatherback Turtle</v>
           </cell>
         </row>
         <row r="40">
           <cell r="C40" t="str">
-            <v>Bat-Eared Fox</v>
+            <v>Pronghorn</v>
           </cell>
         </row>
         <row r="41">
           <cell r="C41" t="str">
-            <v>Greater Flamingo</v>
+            <v xml:space="preserve">Howler Monkey </v>
           </cell>
         </row>
         <row r="42">
           <cell r="C42" t="str">
-            <v>Owl Monkey</v>
+            <v>Coral Snake</v>
           </cell>
         </row>
         <row r="43">
           <cell r="C43" t="str">
-            <v>Caspian Terns</v>
+            <v>Opossum</v>
           </cell>
         </row>
         <row r="44">
           <cell r="C44" t="str">
-            <v>Dyak Fruit Bat</v>
+            <v>Hognose Snake</v>
           </cell>
         </row>
         <row r="45">
           <cell r="C45" t="str">
-            <v>Spotted sandpiper</v>
+            <v>Flame Bowerbird</v>
           </cell>
         </row>
         <row r="46">
           <cell r="C46" t="str">
-            <v>Peacock Wrasse</v>
+            <v>Swamp Nightjar</v>
           </cell>
         </row>
         <row r="47">
           <cell r="C47" t="str">
-            <v>Darwin's Frogs</v>
+            <v>Wrinkle-faced Bat</v>
           </cell>
         </row>
         <row r="48">
           <cell r="C48" t="str">
-            <v>Giant Water Bug</v>
+            <v>Singing Mouse</v>
           </cell>
         </row>
         <row r="49">
           <cell r="C49" t="str">
-            <v xml:space="preserve">Three-Spined stickleback </v>
+            <v>Elegant Dancing Frog</v>
           </cell>
         </row>
         <row r="50">
           <cell r="C50" t="str">
-            <v>Lined Seahorse</v>
+            <v>Honey Bee</v>
           </cell>
         </row>
         <row r="51">
           <cell r="C51" t="str">
-            <v>Golden Eagle</v>
+            <v>Asian Cornborer Moth</v>
           </cell>
         </row>
         <row r="52">
           <cell r="C52" t="str">
-            <v>Cathedral Termite</v>
+            <v>Kob</v>
           </cell>
         </row>
         <row r="53">
           <cell r="C53" t="str">
-            <v>Homo habilis</v>
+            <v>Great Skua</v>
           </cell>
         </row>
         <row r="54">
           <cell r="C54" t="str">
-            <v>Lungfish</v>
+            <v>Porcupine</v>
           </cell>
         </row>
         <row r="55">
           <cell r="C55" t="str">
-            <v>Palaeocastor</v>
+            <v>Koala</v>
           </cell>
         </row>
         <row r="56">
           <cell r="C56" t="str">
-            <v>Goanna</v>
+            <v>Tufted Ground Squirrel</v>
           </cell>
         </row>
         <row r="57">
           <cell r="C57" t="str">
-            <v>Montezuma Oropendola</v>
+            <v>Fork-marked Lemur</v>
           </cell>
         </row>
         <row r="58">
           <cell r="C58" t="str">
-            <v>Veined Octopus</v>
+            <v>Pitcher Plant</v>
           </cell>
         </row>
         <row r="59">
           <cell r="C59" t="str">
-            <v>Puffer Fish</v>
+            <v>Chestnut-headed Bee-eater</v>
           </cell>
         </row>
         <row r="60">
           <cell r="C60" t="str">
-            <v>New Caledonian Crow</v>
+            <v>Hairy-legged Bee</v>
           </cell>
         </row>
         <row r="61">
           <cell r="C61" t="str">
-            <v>Rufous Hornero</v>
+            <v>Northern Short-tailed Shrew</v>
           </cell>
         </row>
         <row r="62">
           <cell r="C62" t="str">
-            <v>Trapdoor Spider</v>
+            <v>Batfly</v>
           </cell>
         </row>
         <row r="63">
           <cell r="C63" t="str">
-            <v>Tent-making Bat</v>
+            <v>Wichita Mountains Pillsnail</v>
           </cell>
         </row>
         <row r="64">
           <cell r="C64" t="str">
-            <v>Bee</v>
+            <v>Cobra Lily</v>
           </cell>
         </row>
         <row r="65">
           <cell r="C65" t="str">
-            <v>Dung Beetle</v>
+            <v>Velvet Worm</v>
           </cell>
         </row>
         <row r="66">
           <cell r="C66" t="str">
-            <v>Spongilla Fly</v>
+            <v>Parasitic Guest Ant</v>
+          </cell>
+        </row>
+        <row r="67">
+          <cell r="C67" t="str">
+            <v>Bear's Head</v>
           </cell>
         </row>
       </sheetData>
@@ -983,19 +1015,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF535796-3E81-4006-B204-DF282F130184}">
   <dimension ref="A1:D67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D67" sqref="D67"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="36.109375"/>
-    <col min="2" max="2" customWidth="true" width="41.33203125"/>
-    <col min="3" max="3" customWidth="true" width="18.44140625"/>
+    <col min="1" max="1" customWidth="true" width="36.140625"/>
+    <col min="2" max="2" customWidth="true" width="41.28515625"/>
+    <col min="3" max="3" customWidth="true" width="18.42578125"/>
     <col min="4" max="4" customWidth="true" width="25.0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1009,10 +1041,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="str">
-        <f>[1]Sheet1!C17</f>
-        <v>Bumblebee Bat</v>
+        <f>[1]Sheet1!C34</f>
+        <v>Sparklemuffin Peacock Spider</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -1021,14 +1053,14 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="str">
-        <f>[1]Sheet1!C19</f>
-        <v>Okapi</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C3</f>
+        <v xml:space="preserve">Sperm Whale </v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="str">
-        <f>[1]Sheet1!C18</f>
-        <v>Shrew Mole</v>
+        <f>[1]Sheet1!C35</f>
+        <v>Rainbow Grasshopper</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -1037,11 +1069,11 @@
         <v>2</v>
       </c>
       <c r="D3" s="1" t="str">
-        <f>[1]Sheet1!C20</f>
-        <v>Kudu</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C4</f>
+        <v xml:space="preserve">Giant Squid </v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1">
         <v>1</v>
@@ -1050,11 +1082,11 @@
         <v>3</v>
       </c>
       <c r="D4" s="1" t="str">
-        <f>[1]Sheet1!C21</f>
-        <v>Striped hyena</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C5</f>
+        <v>Tiger</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1">
         <v>1</v>
@@ -1063,11 +1095,11 @@
         <v>4</v>
       </c>
       <c r="D5" s="1" t="str">
-        <f>[1]Sheet1!C22</f>
-        <v>Striped dolphin</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C6</f>
+        <v>Wolf</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1">
         <v>1</v>
@@ -1076,11 +1108,11 @@
         <v>5</v>
       </c>
       <c r="D6" s="1" t="str">
-        <f>[1]Sheet1!C23</f>
-        <v>Side-striped jackal</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C7</f>
+        <v>Stag</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1">
         <v>1</v>
@@ -1089,11 +1121,11 @@
         <v>6</v>
       </c>
       <c r="D7" s="1" t="str">
-        <f>[1]Sheet1!C24</f>
-        <v>Wildcat</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C8</f>
+        <v>Boar</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1">
         <v>1</v>
@@ -1102,11 +1134,11 @@
         <v>7</v>
       </c>
       <c r="D8" s="1" t="str">
-        <f>[1]Sheet1!C25</f>
-        <v>Striped Rabbit</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C9</f>
+        <v xml:space="preserve">Lucy </v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1">
         <v>1</v>
@@ -1115,11 +1147,11 @@
         <v>8</v>
       </c>
       <c r="D9" s="1" t="str">
-        <f>[1]Sheet1!C26</f>
-        <v>Striped Polecat</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C10</f>
+        <v xml:space="preserve">Raven </v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1">
         <v>1</v>
@@ -1128,11 +1160,11 @@
         <v>9</v>
       </c>
       <c r="D10" s="1" t="str">
-        <f>[1]Sheet1!C27</f>
-        <v>Giant striped mongoose</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C11</f>
+        <v>Wandering Albatross</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1">
         <v>1</v>
@@ -1141,11 +1173,11 @@
         <v>10</v>
       </c>
       <c r="D11" s="1" t="str">
-        <f>[1]Sheet1!C28</f>
-        <v>Numbat</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C12</f>
+        <v>Bigeye Houndshark</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1">
         <v>1</v>
@@ -1154,11 +1186,11 @@
         <v>11</v>
       </c>
       <c r="D12" s="1" t="str">
-        <f>[1]Sheet1!C29</f>
-        <v>Highland Streaked Tenrec</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C13</f>
+        <v>Indian Grey Mongoose</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1">
         <v>1</v>
@@ -1167,11 +1199,11 @@
         <v>12</v>
       </c>
       <c r="D13" s="1" t="str">
-        <f>[1]Sheet1!C30</f>
-        <v>Striped Possum</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C14</f>
+        <v>Starling</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1">
         <v>1</v>
@@ -1180,11 +1212,11 @@
         <v>13</v>
       </c>
       <c r="D14" s="1" t="str">
-        <f>[1]Sheet1!C31</f>
-        <v>Chequered elephant shrew</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C15</f>
+        <v>Harvest Mouse</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1">
         <v>1</v>
@@ -1193,11 +1225,11 @@
         <v>14</v>
       </c>
       <c r="D15" s="1" t="str">
-        <f>[1]Sheet1!C32</f>
-        <v>Fire-footed Rope Squirrel</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C16</f>
+        <v>Catfish</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1">
         <v>1</v>
@@ -1206,11 +1238,11 @@
         <v>15</v>
       </c>
       <c r="D16" s="1" t="str">
-        <f>[1]Sheet1!C33</f>
-        <v>Badger Bat</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C17</f>
+        <v>Tarzan Chameleon</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1">
         <v>1</v>
@@ -1219,11 +1251,11 @@
         <v>16</v>
       </c>
       <c r="D17" s="1" t="str">
-        <f>[1]Sheet1!C34</f>
-        <v>Four-Striped Grass Mouse</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C18</f>
+        <v>Schizomid</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1">
         <v>2</v>
@@ -1232,11 +1264,11 @@
         <v>1</v>
       </c>
       <c r="D18" s="1" t="str">
-        <f>[1]Sheet1!C2</f>
-        <v>Sea Otter</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C19</f>
+        <v>Painted Wild Dog</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1">
         <v>2</v>
@@ -1245,11 +1277,11 @@
         <v>2</v>
       </c>
       <c r="D19" s="1" t="str">
-        <f>[1]Sheet1!C3</f>
-        <v xml:space="preserve">Rock Hyrax </v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C20</f>
+        <v>Red-shanked Douc</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1">
         <v>2</v>
@@ -1258,11 +1290,11 @@
         <v>3</v>
       </c>
       <c r="D20" s="1" t="str">
-        <f>[1]Sheet1!C4</f>
-        <v>Dik Dik</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C21</f>
+        <v>Wolf's Mona Monkey</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1">
         <v>2</v>
@@ -1271,11 +1303,11 @@
         <v>4</v>
       </c>
       <c r="D21" s="1" t="str">
-        <f>[1]Sheet1!C5</f>
-        <v>Mara</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C22</f>
+        <v>Marbled Polecat</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1">
         <v>2</v>
@@ -1284,11 +1316,11 @@
         <v>5</v>
       </c>
       <c r="D22" s="1" t="str">
-        <f>[1]Sheet1!C6</f>
-        <v>Sibree Dwarf Lemur</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C23</f>
+        <v>Halloween Crab</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1">
         <v>2</v>
@@ -1297,11 +1329,11 @@
         <v>6</v>
       </c>
       <c r="D23" s="1" t="str">
-        <f>[1]Sheet1!C7</f>
-        <v>Itjaritjari</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C24</f>
+        <v xml:space="preserve">Peacock Mantis Shrimp </v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1">
         <v>2</v>
@@ -1310,11 +1342,11 @@
         <v>7</v>
       </c>
       <c r="D24" s="1" t="str">
-        <f>[1]Sheet1!C8</f>
-        <v>Bulldog Bat</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C25</f>
+        <v xml:space="preserve">Golden-headed Lion Tamarin </v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1">
         <v>2</v>
@@ -1323,11 +1355,11 @@
         <v>8</v>
       </c>
       <c r="D25" s="1" t="str">
-        <f>[1]Sheet1!C9</f>
-        <v>Southern Ningaui</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C26</f>
+        <v>Himalayan Monal</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1">
         <v>2</v>
@@ -1336,11 +1368,11 @@
         <v>9</v>
       </c>
       <c r="D26" s="1" t="str">
-        <f>[1]Sheet1!C10</f>
-        <v>Grasshopper Mouse</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C27</f>
+        <v>Nicobar Pigeon</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1">
         <v>2</v>
@@ -1349,11 +1381,11 @@
         <v>10</v>
       </c>
       <c r="D27" s="1" t="str">
-        <f>[1]Sheet1!C11</f>
-        <v>Thor's Hero Shrew</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C28</f>
+        <v>Mottled Cup Moth</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1">
         <v>2</v>
@@ -1362,11 +1394,11 @@
         <v>11</v>
       </c>
       <c r="D28" s="1" t="str">
-        <f>[1]Sheet1!C12</f>
-        <v>Silky Anteater</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C29</f>
+        <v>Mandarin Fish</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1">
         <v>2</v>
@@ -1375,11 +1407,11 @@
         <v>12</v>
       </c>
       <c r="D29" s="1" t="str">
-        <f>[1]Sheet1!C13</f>
-        <v>Silver Pika</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C30</f>
+        <v>Bornean Rainbow Toad</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1">
         <v>2</v>
@@ -1388,11 +1420,11 @@
         <v>13</v>
       </c>
       <c r="D30" s="1" t="str">
-        <f>[1]Sheet1!C14</f>
-        <v>Siberian Chipmunk</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C31</f>
+        <v>Madagascan Sunset Moth</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1">
         <v>2</v>
@@ -1401,11 +1433,11 @@
         <v>14</v>
       </c>
       <c r="D31" s="1" t="str">
-        <f>[1]Sheet1!C15</f>
-        <v>Colo Colo Opossum</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C32</f>
+        <v>Flat Lizard</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1">
         <v>2</v>
@@ -1414,11 +1446,11 @@
         <v>15</v>
       </c>
       <c r="D32" s="1" t="str">
-        <f>[1]Sheet1!C16</f>
-        <v>Pygmy Jerboa</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C33</f>
+        <v>Rainbow Scarab</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1">
         <v>2</v>
@@ -1427,11 +1459,11 @@
         <v>16</v>
       </c>
       <c r="D33" s="1" t="str">
-        <f>[1]Sheet1!C17</f>
-        <v>Bumblebee Bat</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C34</f>
+        <v>Sparklemuffin Peacock Spider</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1">
         <v>2</v>
@@ -1440,11 +1472,11 @@
         <v>16</v>
       </c>
       <c r="D34" s="1" t="str">
-        <f>[1]Sheet1!C18</f>
-        <v>Shrew Mole</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C35</f>
+        <v>Rainbow Grasshopper</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1">
         <v>3</v>
@@ -1453,11 +1485,11 @@
         <v>1</v>
       </c>
       <c r="D35" s="1" t="str">
-        <f>[1]Sheet1!C51</f>
-        <v>Golden Eagle</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C52</f>
+        <v>Kob</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1">
         <v>3</v>
@@ -1466,11 +1498,11 @@
         <v>2</v>
       </c>
       <c r="D36" s="1" t="str">
-        <f>[1]Sheet1!C52</f>
-        <v>Cathedral Termite</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C53</f>
+        <v>Great Skua</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1">
         <v>3</v>
@@ -1479,11 +1511,11 @@
         <v>3</v>
       </c>
       <c r="D37" s="1" t="str">
-        <f>[1]Sheet1!C53</f>
-        <v>Homo habilis</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C54</f>
+        <v>Porcupine</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1">
         <v>3</v>
@@ -1492,11 +1524,11 @@
         <v>4</v>
       </c>
       <c r="D38" s="1" t="str">
-        <f>[1]Sheet1!C54</f>
-        <v>Lungfish</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C55</f>
+        <v>Koala</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1">
         <v>3</v>
@@ -1505,11 +1537,11 @@
         <v>5</v>
       </c>
       <c r="D39" s="1" t="str">
-        <f>[1]Sheet1!C55</f>
-        <v>Palaeocastor</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C56</f>
+        <v>Tufted Ground Squirrel</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1">
         <v>3</v>
@@ -1518,11 +1550,11 @@
         <v>6</v>
       </c>
       <c r="D40" s="1" t="str">
-        <f>[1]Sheet1!C56</f>
-        <v>Goanna</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C57</f>
+        <v>Fork-marked Lemur</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1">
         <v>3</v>
@@ -1531,11 +1563,11 @@
         <v>7</v>
       </c>
       <c r="D41" s="1" t="str">
-        <f>[1]Sheet1!C57</f>
-        <v>Montezuma Oropendola</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C58</f>
+        <v>Pitcher Plant</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1">
         <v>3</v>
@@ -1544,11 +1576,11 @@
         <v>8</v>
       </c>
       <c r="D42" s="1" t="str">
-        <f>[1]Sheet1!C58</f>
-        <v>Veined Octopus</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C59</f>
+        <v>Chestnut-headed Bee-eater</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1">
         <v>3</v>
@@ -1557,11 +1589,11 @@
         <v>9</v>
       </c>
       <c r="D43" s="1" t="str">
-        <f>[1]Sheet1!C59</f>
-        <v>Puffer Fish</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C60</f>
+        <v>Hairy-legged Bee</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1">
         <v>3</v>
@@ -1570,11 +1602,11 @@
         <v>10</v>
       </c>
       <c r="D44" s="1" t="str">
-        <f>[1]Sheet1!C60</f>
-        <v>New Caledonian Crow</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C61</f>
+        <v>Northern Short-tailed Shrew</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1">
         <v>3</v>
@@ -1583,11 +1615,11 @@
         <v>11</v>
       </c>
       <c r="D45" s="1" t="str">
-        <f>[1]Sheet1!C61</f>
-        <v>Rufous Hornero</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C62</f>
+        <v>Batfly</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1">
         <v>3</v>
@@ -1596,11 +1628,11 @@
         <v>12</v>
       </c>
       <c r="D46" s="1" t="str">
-        <f>[1]Sheet1!C62</f>
-        <v>Trapdoor Spider</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C63</f>
+        <v>Wichita Mountains Pillsnail</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1">
         <v>3</v>
@@ -1609,11 +1641,11 @@
         <v>13</v>
       </c>
       <c r="D47" s="1" t="str">
-        <f>[1]Sheet1!C63</f>
-        <v>Tent-making Bat</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C64</f>
+        <v>Cobra Lily</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1">
         <v>3</v>
@@ -1622,11 +1654,11 @@
         <v>14</v>
       </c>
       <c r="D48" s="1" t="str">
-        <f>[1]Sheet1!C64</f>
-        <v>Bee</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C65</f>
+        <v>Velvet Worm</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1">
         <v>3</v>
@@ -1635,11 +1667,11 @@
         <v>15</v>
       </c>
       <c r="D49" s="1" t="str">
-        <f>[1]Sheet1!C65</f>
-        <v>Dung Beetle</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C66</f>
+        <v>Parasitic Guest Ant</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1">
         <v>3</v>
@@ -1648,11 +1680,11 @@
         <v>16</v>
       </c>
       <c r="D50" s="1" t="str">
-        <f>[1]Sheet1!C66</f>
-        <v>Spongilla Fly</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C67</f>
+        <v>Bear's Head</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1">
         <v>4</v>
@@ -1661,11 +1693,11 @@
         <v>1</v>
       </c>
       <c r="D51" s="1" t="str">
-        <f>[1]Sheet1!C35</f>
-        <v>Emperor Penguin</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C36</f>
+        <v>Northern Elephant Seal</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1">
         <v>4</v>
@@ -1674,11 +1706,11 @@
         <v>2</v>
       </c>
       <c r="D52" s="1" t="str">
-        <f>[1]Sheet1!C36</f>
-        <v>Greater Rhea</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C37</f>
+        <v>Forest Elephant</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="1">
         <v>4</v>
@@ -1687,11 +1719,11 @@
         <v>3</v>
       </c>
       <c r="D53" s="1" t="str">
-        <f>[1]Sheet1!C37</f>
-        <v>Wolverine</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C38</f>
+        <v>Great White Shark</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="1">
         <v>4</v>
@@ -1700,11 +1732,11 @@
         <v>4</v>
       </c>
       <c r="D54" s="1" t="str">
-        <f>[1]Sheet1!C38</f>
-        <v>Siamang</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C39</f>
+        <v>Leatherback Turtle</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="1">
         <v>4</v>
@@ -1713,11 +1745,11 @@
         <v>5</v>
       </c>
       <c r="D55" s="1" t="str">
-        <f>[1]Sheet1!C39</f>
-        <v>Pacific Spiny Lumpsucker</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C40</f>
+        <v>Pronghorn</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="1">
         <v>4</v>
@@ -1726,11 +1758,11 @@
         <v>6</v>
       </c>
       <c r="D56" s="1" t="str">
-        <f>[1]Sheet1!C40</f>
-        <v>Bat-Eared Fox</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C41</f>
+        <v xml:space="preserve">Howler Monkey </v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="1">
         <v>4</v>
@@ -1739,11 +1771,11 @@
         <v>7</v>
       </c>
       <c r="D57" s="1" t="str">
-        <f>[1]Sheet1!C41</f>
-        <v>Greater Flamingo</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C42</f>
+        <v>Coral Snake</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="1">
         <v>4</v>
@@ -1752,11 +1784,11 @@
         <v>8</v>
       </c>
       <c r="D58" s="1" t="str">
-        <f>[1]Sheet1!C42</f>
-        <v>Owl Monkey</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C43</f>
+        <v>Opossum</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="1">
         <v>4</v>
@@ -1765,11 +1797,11 @@
         <v>9</v>
       </c>
       <c r="D59" s="1" t="str">
-        <f>[1]Sheet1!C43</f>
-        <v>Caspian Terns</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C44</f>
+        <v>Hognose Snake</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1">
         <v>4</v>
@@ -1778,11 +1810,11 @@
         <v>10</v>
       </c>
       <c r="D60" s="1" t="str">
-        <f>[1]Sheet1!C44</f>
-        <v>Dyak Fruit Bat</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C45</f>
+        <v>Flame Bowerbird</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="1">
         <v>4</v>
@@ -1791,11 +1823,11 @@
         <v>11</v>
       </c>
       <c r="D61" s="1" t="str">
-        <f>[1]Sheet1!C45</f>
-        <v>Spotted sandpiper</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C46</f>
+        <v>Swamp Nightjar</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1">
         <v>4</v>
@@ -1804,11 +1836,11 @@
         <v>12</v>
       </c>
       <c r="D62" s="1" t="str">
-        <f>[1]Sheet1!C46</f>
-        <v>Peacock Wrasse</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C47</f>
+        <v>Wrinkle-faced Bat</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="1">
         <v>4</v>
@@ -1817,11 +1849,11 @@
         <v>13</v>
       </c>
       <c r="D63" s="1" t="str">
-        <f>[1]Sheet1!C47</f>
-        <v>Darwin's Frogs</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C48</f>
+        <v>Singing Mouse</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="1">
         <v>4</v>
@@ -1830,11 +1862,11 @@
         <v>14</v>
       </c>
       <c r="D64" s="1" t="str">
-        <f>[1]Sheet1!C48</f>
-        <v>Giant Water Bug</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C49</f>
+        <v>Elegant Dancing Frog</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="1">
         <v>4</v>
@@ -1843,11 +1875,11 @@
         <v>15</v>
       </c>
       <c r="D65" s="1" t="str">
-        <f>[1]Sheet1!C49</f>
-        <v xml:space="preserve">Three-Spined stickleback </v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C50</f>
+        <v>Honey Bee</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="1">
         <v>4</v>
@@ -1856,16 +1888,17 @@
         <v>16</v>
       </c>
       <c r="D66" s="1" t="str">
-        <f>[1]Sheet1!C50</f>
-        <v>Lined Seahorse</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+        <f>[1]Sheet1!C51</f>
+        <v>Asian Cornborer Moth</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D67" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1877,27 +1910,27 @@
       <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="14.6640625"/>
-    <col min="3" max="3" customWidth="true" width="25.44140625"/>
-    <col min="15" max="15" customWidth="true" width="23.44140625"/>
+    <col min="2" max="2" customWidth="true" width="14.7109375"/>
+    <col min="3" max="3" customWidth="true" width="25.42578125"/>
+    <col min="15" max="15" customWidth="true" width="23.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="0">
         <v>0</v>
       </c>
       <c r="C1" t="str" s="0">
         <f>Helper!D2</f>
-        <v>Okapi</v>
+        <v xml:space="preserve">Sperm Whale </v>
       </c>
       <c r="O1" t="str" s="0">
         <f>Helper!D35</f>
-        <v>Golden Eagle</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Kob</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="0">
         <v>1</v>
       </c>
@@ -1908,20 +1941,20 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="0">
         <v>2</v>
       </c>
       <c r="C3" t="str" s="0">
         <f>Helper!D17</f>
-        <v>Four-Striped Grass Mouse</v>
+        <v>Schizomid</v>
       </c>
       <c r="O3" t="str" s="0">
         <f>Helper!D50</f>
-        <v>Spongilla Fly</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Bear's Head</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="0">
         <v>3</v>
       </c>
@@ -1932,20 +1965,20 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="0">
         <v>4</v>
       </c>
       <c r="C5" t="str" s="0">
         <f>Helper!D9</f>
-        <v>Striped Polecat</v>
+        <v xml:space="preserve">Raven </v>
       </c>
       <c r="O5" t="str" s="0">
         <f>Helper!D42</f>
-        <v>Veined Octopus</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Chestnut-headed Bee-eater</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="0">
         <v>5</v>
       </c>
@@ -1956,20 +1989,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="0">
         <v>6</v>
       </c>
       <c r="C7" t="str" s="0">
         <f>Helper!D10</f>
-        <v>Giant striped mongoose</v>
+        <v>Wandering Albatross</v>
       </c>
       <c r="O7" t="str" s="0">
         <f>Helper!D43</f>
-        <v>Puffer Fish</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Hairy-legged Bee</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="0">
         <v>7</v>
       </c>
@@ -1980,20 +2013,20 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="0">
         <v>8</v>
       </c>
       <c r="C9" t="str" s="0">
         <f>Helper!D6</f>
-        <v>Side-striped jackal</v>
+        <v>Stag</v>
       </c>
       <c r="O9" t="str" s="0">
         <f>Helper!D39</f>
-        <v>Palaeocastor</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Tufted Ground Squirrel</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="0">
         <v>9</v>
       </c>
@@ -2004,20 +2037,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="0">
         <v>10</v>
       </c>
       <c r="C11" t="str" s="0">
         <f>Helper!D13</f>
-        <v>Striped Possum</v>
+        <v>Starling</v>
       </c>
       <c r="O11" t="str" s="0">
         <f>Helper!D46</f>
-        <v>Trapdoor Spider</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Wichita Mountains Pillsnail</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="0">
         <v>11</v>
       </c>
@@ -2028,20 +2061,20 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="0">
         <v>12</v>
       </c>
       <c r="C13" t="str" s="0">
         <f>Helper!D5</f>
-        <v>Striped dolphin</v>
+        <v>Wolf</v>
       </c>
       <c r="O13" t="str" s="0">
         <f>Helper!D38</f>
-        <v>Lungfish</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Koala</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="0">
         <v>13</v>
       </c>
@@ -2052,20 +2085,20 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="0">
         <v>14</v>
       </c>
       <c r="C15" t="str" s="0">
         <f>Helper!D14</f>
-        <v>Chequered elephant shrew</v>
+        <v>Harvest Mouse</v>
       </c>
       <c r="O15" t="str" s="0">
         <f>Helper!D47</f>
-        <v>Tent-making Bat</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Cobra Lily</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="0">
         <v>15</v>
       </c>
@@ -2076,20 +2109,20 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="0">
         <v>16</v>
       </c>
       <c r="C17" t="str" s="0">
         <f>Helper!D7</f>
-        <v>Wildcat</v>
+        <v>Boar</v>
       </c>
       <c r="O17" t="str" s="0">
         <f>Helper!D40</f>
-        <v>Goanna</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Fork-marked Lemur</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="0">
         <v>17</v>
       </c>
@@ -2100,20 +2133,20 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="0">
         <v>18</v>
       </c>
       <c r="C19" t="str" s="0">
         <f>Helper!D12</f>
-        <v>Highland Streaked Tenrec</v>
+        <v>Indian Grey Mongoose</v>
       </c>
       <c r="O19" t="str" s="0">
         <f>Helper!D45</f>
-        <v>Rufous Hornero</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Batfly</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="0">
         <v>19</v>
       </c>
@@ -2124,20 +2157,20 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="0">
         <v>20</v>
       </c>
       <c r="C21" t="str" s="0">
         <f>Helper!D4</f>
-        <v>Striped hyena</v>
+        <v>Tiger</v>
       </c>
       <c r="O21" t="str" s="0">
         <f>Helper!D37</f>
-        <v>Homo habilis</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Porcupine</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="0">
         <v>21</v>
       </c>
@@ -2148,20 +2181,20 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="0">
         <v>22</v>
       </c>
       <c r="C23" t="str" s="0">
         <f>Helper!D15</f>
-        <v>Fire-footed Rope Squirrel</v>
+        <v>Catfish</v>
       </c>
       <c r="O23" t="str" s="0">
         <f>Helper!D48</f>
-        <v>Bee</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Velvet Worm</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="0">
         <v>23</v>
       </c>
@@ -2172,20 +2205,20 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="0">
         <v>24</v>
       </c>
       <c r="C25" t="str" s="0">
         <f>Helper!D8</f>
-        <v>Striped Rabbit</v>
+        <v xml:space="preserve">Lucy </v>
       </c>
       <c r="O25" t="str" s="0">
         <f>Helper!D41</f>
-        <v>Montezuma Oropendola</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Pitcher Plant</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="0">
         <v>25</v>
       </c>
@@ -2196,20 +2229,20 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="0">
         <v>26</v>
       </c>
       <c r="C27" t="str" s="0">
         <f>Helper!D11</f>
-        <v>Numbat</v>
+        <v>Bigeye Houndshark</v>
       </c>
       <c r="O27" t="str" s="0">
         <f>Helper!D44</f>
-        <v>New Caledonian Crow</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Northern Short-tailed Shrew</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="0">
         <v>27</v>
       </c>
@@ -2220,20 +2253,20 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="0">
         <v>28</v>
       </c>
       <c r="C29" t="str" s="0">
         <f>Helper!D3</f>
-        <v>Kudu</v>
+        <v xml:space="preserve">Giant Squid </v>
       </c>
       <c r="O29" t="str" s="0">
         <f>Helper!D36</f>
-        <v>Cathedral Termite</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Great Skua</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="0">
         <v>29</v>
       </c>
@@ -2244,20 +2277,20 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="0">
         <v>30</v>
       </c>
       <c r="C31" t="str" s="0">
         <f>Helper!D16</f>
-        <v>Badger Bat</v>
+        <v>Tarzan Chameleon</v>
       </c>
       <c r="O31" t="str" s="0">
         <f>Helper!D49</f>
-        <v>Dung Beetle</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Parasitic Guest Ant</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="0">
         <v>31</v>
       </c>
@@ -2271,26 +2304,26 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="0">
         <v>32</v>
       </c>
       <c r="C33" t="str" s="0">
         <f>Helper!D18</f>
-        <v>Sea Otter</v>
+        <v>Painted Wild Dog</v>
       </c>
       <c r="O33" t="str" s="0">
         <f>Helper!D51</f>
-        <v>Emperor Penguin</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Northern Elephant Seal</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="0">
         <v>33</v>
       </c>
       <c r="B34" t="str" s="0">
         <f>Helper!A2</f>
-        <v>Bumblebee Bat</v>
+        <v>Sparklemuffin Peacock Spider</v>
       </c>
       <c r="D34" t="s" s="0">
         <v>4</v>
@@ -2299,7 +2332,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="0">
         <v>34</v>
       </c>
@@ -2308,16 +2341,16 @@
       </c>
       <c r="O35" t="str" s="0">
         <f>Helper!D66</f>
-        <v>Lined Seahorse</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Asian Cornborer Moth</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="0">
         <v>35</v>
       </c>
       <c r="B36" t="str" s="0">
         <f>Helper!A3</f>
-        <v>Shrew Mole</v>
+        <v>Rainbow Grasshopper</v>
       </c>
       <c r="E36" t="s" s="0">
         <v>4</v>
@@ -2326,20 +2359,20 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="0">
         <v>36</v>
       </c>
       <c r="C37" t="str" s="0">
         <f>Helper!D25</f>
-        <v>Southern Ningaui</v>
+        <v>Himalayan Monal</v>
       </c>
       <c r="O37" t="str" s="0">
         <f>Helper!D58</f>
-        <v>Owl Monkey</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Opossum</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="0">
         <v>37</v>
       </c>
@@ -2350,20 +2383,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="0">
         <v>38</v>
       </c>
       <c r="C39" t="str" s="0">
         <f>Helper!D26</f>
-        <v>Grasshopper Mouse</v>
+        <v>Nicobar Pigeon</v>
       </c>
       <c r="O39" t="str" s="0">
         <f>Helper!D59</f>
-        <v>Caspian Terns</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Hognose Snake</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="0">
         <v>39</v>
       </c>
@@ -2374,20 +2407,20 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="0">
         <v>40</v>
       </c>
       <c r="C41" t="str" s="0">
         <f>Helper!D22</f>
-        <v>Sibree Dwarf Lemur</v>
+        <v>Halloween Crab</v>
       </c>
       <c r="O41" t="str" s="0">
         <f>Helper!D55</f>
-        <v>Pacific Spiny Lumpsucker</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Pronghorn</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="0">
         <v>41</v>
       </c>
@@ -2398,20 +2431,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="0">
         <v>42</v>
       </c>
       <c r="C43" t="str" s="0">
         <f>Helper!D29</f>
-        <v>Silver Pika</v>
+        <v>Bornean Rainbow Toad</v>
       </c>
       <c r="O43" t="str" s="0">
         <f>Helper!D62</f>
-        <v>Peacock Wrasse</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Wrinkle-faced Bat</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="0">
         <v>43</v>
       </c>
@@ -2422,20 +2455,20 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="0">
         <v>44</v>
       </c>
       <c r="C45" t="str" s="0">
         <f>Helper!D21</f>
-        <v>Mara</v>
+        <v>Marbled Polecat</v>
       </c>
       <c r="O45" t="str" s="0">
         <f>Helper!D54</f>
-        <v>Siamang</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Leatherback Turtle</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="0">
         <v>45</v>
       </c>
@@ -2446,20 +2479,20 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="0">
         <v>46</v>
       </c>
       <c r="C47" t="str" s="0">
         <f>Helper!D30</f>
-        <v>Siberian Chipmunk</v>
+        <v>Madagascan Sunset Moth</v>
       </c>
       <c r="O47" t="str" s="0">
         <f>Helper!D63</f>
-        <v>Darwin's Frogs</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Singing Mouse</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="0">
         <v>47</v>
       </c>
@@ -2470,20 +2503,20 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" s="0">
         <v>48</v>
       </c>
       <c r="C49" t="str" s="0">
         <f>Helper!D23</f>
-        <v>Itjaritjari</v>
+        <v xml:space="preserve">Peacock Mantis Shrimp </v>
       </c>
       <c r="O49" t="str" s="0">
         <f>Helper!D56</f>
-        <v>Bat-Eared Fox</v>
-      </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+        <v xml:space="preserve">Howler Monkey </v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" s="0">
         <v>49</v>
       </c>
@@ -2494,20 +2527,20 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" s="0">
         <v>50</v>
       </c>
       <c r="C51" t="str" s="0">
         <f>Helper!D28</f>
-        <v>Silky Anteater</v>
+        <v>Mandarin Fish</v>
       </c>
       <c r="O51" t="str" s="0">
         <f>Helper!D61</f>
-        <v>Spotted sandpiper</v>
-      </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Swamp Nightjar</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" s="0">
         <v>51</v>
       </c>
@@ -2518,20 +2551,20 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" s="0">
         <v>52</v>
       </c>
       <c r="C53" t="str" s="0">
         <f>Helper!D20</f>
-        <v>Dik Dik</v>
+        <v>Wolf's Mona Monkey</v>
       </c>
       <c r="O53" t="str" s="0">
         <f>Helper!D53</f>
-        <v>Wolverine</v>
-      </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Great White Shark</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" s="0">
         <v>53</v>
       </c>
@@ -2542,20 +2575,20 @@
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" s="0">
         <v>54</v>
       </c>
       <c r="C55" t="str" s="0">
         <f>Helper!D31</f>
-        <v>Colo Colo Opossum</v>
+        <v>Flat Lizard</v>
       </c>
       <c r="O55" t="str" s="0">
         <f>Helper!D64</f>
-        <v>Giant Water Bug</v>
-      </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Elegant Dancing Frog</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" s="0">
         <v>55</v>
       </c>
@@ -2566,20 +2599,20 @@
         <v>11</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="0">
         <v>56</v>
       </c>
       <c r="C57" t="str" s="0">
         <f>Helper!D24</f>
-        <v>Bulldog Bat</v>
+        <v xml:space="preserve">Golden-headed Lion Tamarin </v>
       </c>
       <c r="O57" t="str" s="0">
         <f>Helper!D57</f>
-        <v>Greater Flamingo</v>
-      </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Coral Snake</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" s="0">
         <v>57</v>
       </c>
@@ -2590,20 +2623,20 @@
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" s="0">
         <v>58</v>
       </c>
       <c r="C59" t="str" s="0">
         <f>Helper!D27</f>
-        <v>Thor's Hero Shrew</v>
+        <v>Mottled Cup Moth</v>
       </c>
       <c r="O59" t="str" s="0">
         <f>Helper!D60</f>
-        <v>Dyak Fruit Bat</v>
-      </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Flame Bowerbird</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" s="0">
         <v>59</v>
       </c>
@@ -2614,20 +2647,20 @@
         <v>11</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" s="0">
         <v>60</v>
       </c>
       <c r="C61" t="str" s="0">
         <f>Helper!D19</f>
-        <v xml:space="preserve">Rock Hyrax </v>
+        <v>Red-shanked Douc</v>
       </c>
       <c r="O61" t="str" s="0">
         <f>Helper!D52</f>
-        <v>Greater Rhea</v>
-      </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Forest Elephant</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" s="0">
         <v>61</v>
       </c>
@@ -2638,21 +2671,21 @@
         <v>11</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" s="0">
         <v>62</v>
       </c>
       <c r="C63" t="str" s="0">
         <f>Helper!D32</f>
-        <v>Pygmy Jerboa</v>
+        <v>Rainbow Scarab</v>
       </c>
       <c r="O63" t="str" s="0">
         <f>Helper!D65</f>
-        <v xml:space="preserve">Three-Spined stickleback </v>
+        <v>Honey Bee</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:O64">
+  <sortState ref="A1:O64">
     <sortCondition ref="A1:A64"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2663,781 +2696,781 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97DD84F6-D856-4FCA-9254-65D9DBB06268}">
   <dimension ref="A1:O63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D38" zoomScale="56" zoomScaleNormal="39" workbookViewId="0">
+    <sheetView topLeftCell="D38" zoomScale="56" zoomScaleNormal="39" workbookViewId="0">
       <selection activeCell="N61" sqref="N61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="14.6640625"/>
-    <col min="3" max="15" customWidth="true" width="23.6640625"/>
+    <col min="2" max="2" customWidth="true" width="14.7109375"/>
+    <col min="3" max="15" customWidth="true" width="23.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="0">
         <v>0</v>
       </c>
       <c r="C1" t="str" s="0">
         <f>Helper!D2</f>
-        <v>Okapi</v>
+        <v xml:space="preserve">Sperm Whale </v>
       </c>
       <c r="O1" t="str" s="0">
         <f>Helper!D35</f>
-        <v>Golden Eagle</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Kob</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="0">
         <v>1</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="N2" t="s" s="0">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="0">
         <v>2</v>
       </c>
       <c r="C3" t="str" s="0">
         <f>Helper!D17</f>
-        <v>Four-Striped Grass Mouse</v>
+        <v>Schizomid</v>
       </c>
       <c r="O3" t="str" s="0">
         <f>Helper!D50</f>
-        <v>Spongilla Fly</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Bear's Head</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="0">
         <v>3</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="M4" t="s" s="0">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="0">
         <v>4</v>
       </c>
       <c r="C5" t="str" s="0">
         <f>Helper!D9</f>
-        <v>Striped Polecat</v>
+        <v xml:space="preserve">Raven </v>
       </c>
       <c r="O5" t="str" s="0">
         <f>Helper!D42</f>
-        <v>Veined Octopus</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Chestnut-headed Bee-eater</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="0">
         <v>5</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="N6" t="s" s="0">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="0">
         <v>6</v>
       </c>
       <c r="C7" t="str" s="0">
         <f>Helper!D10</f>
-        <v>Giant striped mongoose</v>
+        <v>Wandering Albatross</v>
       </c>
       <c r="O7" t="str" s="0">
         <f>Helper!D43</f>
-        <v>Puffer Fish</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Hairy-legged Bee</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="0">
         <v>7</v>
       </c>
       <c r="F8" t="s" s="0">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="L8" t="s" s="0">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="0">
         <v>8</v>
       </c>
       <c r="C9" t="str" s="0">
         <f>Helper!D6</f>
-        <v>Side-striped jackal</v>
+        <v>Stag</v>
       </c>
       <c r="O9" t="str" s="0">
         <f>Helper!D39</f>
-        <v>Palaeocastor</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Tufted Ground Squirrel</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="0">
         <v>9</v>
       </c>
       <c r="D10" t="s" s="0">
-        <v>50</v>
+        <v>82</v>
       </c>
       <c r="N10" t="s" s="0">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="0">
         <v>10</v>
       </c>
       <c r="C11" t="str" s="0">
         <f>Helper!D13</f>
-        <v>Striped Possum</v>
+        <v>Starling</v>
       </c>
       <c r="O11" t="str" s="0">
         <f>Helper!D46</f>
-        <v>Trapdoor Spider</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Wichita Mountains Pillsnail</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="0">
         <v>11</v>
       </c>
       <c r="E12" t="s" s="0">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="M12" t="s" s="0">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="0">
         <v>12</v>
       </c>
       <c r="C13" t="str" s="0">
         <f>Helper!D5</f>
-        <v>Striped dolphin</v>
+        <v>Wolf</v>
       </c>
       <c r="O13" t="str" s="0">
         <f>Helper!D38</f>
-        <v>Lungfish</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Koala</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="0">
         <v>13</v>
       </c>
       <c r="D14" t="s" s="0">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="N14" t="s" s="0">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="0">
         <v>14</v>
       </c>
       <c r="C15" t="str" s="0">
         <f>Helper!D14</f>
-        <v>Chequered elephant shrew</v>
+        <v>Harvest Mouse</v>
       </c>
       <c r="O15" t="str" s="0">
         <f>Helper!D47</f>
-        <v>Tent-making Bat</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Cobra Lily</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="0">
         <v>15</v>
       </c>
       <c r="G16" t="s" s="0">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="K16" t="s" s="0">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="0">
         <v>16</v>
       </c>
       <c r="C17" t="str" s="0">
         <f>Helper!D7</f>
-        <v>Wildcat</v>
+        <v>Boar</v>
       </c>
       <c r="O17" t="str" s="0">
         <f>Helper!D40</f>
-        <v>Goanna</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Fork-marked Lemur</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="0">
         <v>17</v>
       </c>
       <c r="D18" t="s" s="0">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="N18" t="s" s="0">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="0">
         <v>18</v>
       </c>
       <c r="C19" t="str" s="0">
         <f>Helper!D12</f>
-        <v>Highland Streaked Tenrec</v>
+        <v>Indian Grey Mongoose</v>
       </c>
       <c r="O19" t="str" s="0">
         <f>Helper!D45</f>
-        <v>Rufous Hornero</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Batfly</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="0">
         <v>19</v>
       </c>
       <c r="E20" t="s" s="0">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="M20" t="s" s="0">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="0">
         <v>20</v>
       </c>
       <c r="C21" t="str" s="0">
         <f>Helper!D4</f>
-        <v>Striped hyena</v>
+        <v>Tiger</v>
       </c>
       <c r="O21" t="str" s="0">
         <f>Helper!D37</f>
-        <v>Homo habilis</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Porcupine</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="0">
         <v>21</v>
       </c>
       <c r="D22" t="s" s="0">
-        <v>17</v>
+        <v>83</v>
       </c>
       <c r="N22" t="s" s="0">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="0">
         <v>22</v>
       </c>
       <c r="C23" t="str" s="0">
         <f>Helper!D15</f>
-        <v>Fire-footed Rope Squirrel</v>
+        <v>Catfish</v>
       </c>
       <c r="O23" t="str" s="0">
         <f>Helper!D48</f>
-        <v>Bee</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Velvet Worm</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="0">
         <v>23</v>
       </c>
       <c r="F24" t="s" s="0">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="L24" t="s" s="0">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="0">
         <v>24</v>
       </c>
       <c r="C25" t="str" s="0">
         <f>Helper!D8</f>
-        <v>Striped Rabbit</v>
+        <v xml:space="preserve">Lucy </v>
       </c>
       <c r="O25" t="str" s="0">
         <f>Helper!D41</f>
-        <v>Montezuma Oropendola</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Pitcher Plant</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="0">
         <v>25</v>
       </c>
       <c r="D26" t="s" s="0">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="N26" t="s" s="0">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="0">
         <v>26</v>
       </c>
       <c r="C27" t="str" s="0">
         <f>Helper!D11</f>
-        <v>Numbat</v>
+        <v>Bigeye Houndshark</v>
       </c>
       <c r="O27" t="str" s="0">
         <f>Helper!D44</f>
-        <v>New Caledonian Crow</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Northern Short-tailed Shrew</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="0">
         <v>27</v>
       </c>
       <c r="E28" t="s" s="0">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="M28" t="s" s="0">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="0">
         <v>28</v>
       </c>
       <c r="C29" t="str" s="0">
         <f>Helper!D3</f>
-        <v>Kudu</v>
+        <v xml:space="preserve">Giant Squid </v>
       </c>
       <c r="O29" t="str" s="0">
         <f>Helper!D36</f>
-        <v>Cathedral Termite</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Great Skua</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="0">
         <v>29</v>
       </c>
       <c r="D30" t="s" s="0">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="N30" t="s" s="0">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="0">
         <v>30</v>
       </c>
       <c r="C31" t="str" s="0">
         <f>Helper!D16</f>
-        <v>Badger Bat</v>
+        <v>Tarzan Chameleon</v>
       </c>
       <c r="O31" t="str" s="0">
         <f>Helper!D49</f>
-        <v>Dung Beetle</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Parasitic Guest Ant</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="0">
         <v>31</v>
       </c>
       <c r="H32" t="s" s="0">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="I32" t="s" s="0">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="J32" t="s" s="0">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="0">
         <v>32</v>
       </c>
       <c r="C33" t="str" s="0">
         <f>Helper!D18</f>
-        <v>Sea Otter</v>
+        <v>Painted Wild Dog</v>
       </c>
       <c r="O33" t="str" s="0">
         <f>Helper!D51</f>
-        <v>Emperor Penguin</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Northern Elephant Seal</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="0">
         <v>33</v>
       </c>
       <c r="B34" t="str" s="0">
         <f>Helper!A2</f>
-        <v>Bumblebee Bat</v>
+        <v>Sparklemuffin Peacock Spider</v>
       </c>
       <c r="D34" t="s" s="0">
-        <v>30</v>
+        <v>84</v>
       </c>
       <c r="N34" t="s" s="0">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="0">
         <v>34</v>
       </c>
       <c r="C35" t="s" s="0">
-        <v>49</v>
+        <v>81</v>
       </c>
       <c r="O35" t="str" s="0">
         <f>Helper!D66</f>
-        <v>Lined Seahorse</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Asian Cornborer Moth</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="0">
         <v>35</v>
       </c>
       <c r="B36" t="str" s="0">
         <f>Helper!A3</f>
-        <v>Shrew Mole</v>
+        <v>Rainbow Grasshopper</v>
       </c>
       <c r="E36" t="s" s="0">
-        <v>30</v>
+        <v>84</v>
       </c>
       <c r="M36" t="s" s="0">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="0">
         <v>36</v>
       </c>
       <c r="C37" t="str" s="0">
         <f>Helper!D25</f>
-        <v>Southern Ningaui</v>
+        <v>Himalayan Monal</v>
       </c>
       <c r="O37" t="str" s="0">
         <f>Helper!D58</f>
-        <v>Owl Monkey</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Opossum</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="0">
         <v>37</v>
       </c>
       <c r="D38" t="s" s="0">
-        <v>32</v>
+        <v>85</v>
       </c>
       <c r="N38" t="s" s="0">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="0">
         <v>38</v>
       </c>
       <c r="C39" t="str" s="0">
         <f>Helper!D26</f>
-        <v>Grasshopper Mouse</v>
+        <v>Nicobar Pigeon</v>
       </c>
       <c r="O39" t="str" s="0">
         <f>Helper!D59</f>
-        <v>Caspian Terns</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Hognose Snake</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="0">
         <v>39</v>
       </c>
       <c r="F40" t="s" s="0">
-        <v>36</v>
+        <v>84</v>
       </c>
       <c r="L40" t="s" s="0">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="0">
         <v>40</v>
       </c>
       <c r="C41" t="str" s="0">
         <f>Helper!D22</f>
-        <v>Sibree Dwarf Lemur</v>
+        <v>Halloween Crab</v>
       </c>
       <c r="O41" t="str" s="0">
         <f>Helper!D55</f>
-        <v>Pacific Spiny Lumpsucker</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Pronghorn</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="0">
         <v>41</v>
       </c>
       <c r="D42" t="s" s="0">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="N42" t="s" s="0">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="0">
         <v>42</v>
       </c>
       <c r="C43" t="str" s="0">
         <f>Helper!D29</f>
-        <v>Silver Pika</v>
+        <v>Bornean Rainbow Toad</v>
       </c>
       <c r="O43" t="str" s="0">
         <f>Helper!D62</f>
-        <v>Peacock Wrasse</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Wrinkle-faced Bat</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="0">
         <v>43</v>
       </c>
       <c r="E44" t="s" s="0">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="M44" t="s" s="0">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="0">
         <v>44</v>
       </c>
       <c r="C45" t="str" s="0">
         <f>Helper!D21</f>
-        <v>Mara</v>
+        <v>Marbled Polecat</v>
       </c>
       <c r="O45" t="str" s="0">
         <f>Helper!D54</f>
-        <v>Siamang</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Leatherback Turtle</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="0">
         <v>45</v>
       </c>
       <c r="D46" t="s" s="0">
-        <v>36</v>
+        <v>86</v>
       </c>
       <c r="N46" t="s" s="0">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="0">
         <v>46</v>
       </c>
       <c r="C47" t="str" s="0">
         <f>Helper!D30</f>
-        <v>Siberian Chipmunk</v>
+        <v>Madagascan Sunset Moth</v>
       </c>
       <c r="O47" t="str" s="0">
         <f>Helper!D63</f>
-        <v>Darwin's Frogs</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Singing Mouse</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="0">
         <v>47</v>
       </c>
       <c r="G48" t="s" s="0">
-        <v>18</v>
+        <v>84</v>
       </c>
       <c r="K48" t="s" s="0">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" s="0">
         <v>48</v>
       </c>
       <c r="C49" t="str" s="0">
         <f>Helper!D23</f>
-        <v>Itjaritjari</v>
+        <v xml:space="preserve">Peacock Mantis Shrimp </v>
       </c>
       <c r="O49" t="str" s="0">
         <f>Helper!D56</f>
-        <v>Bat-Eared Fox</v>
-      </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+        <v xml:space="preserve">Howler Monkey </v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" s="0">
         <v>49</v>
       </c>
       <c r="D50" t="s" s="0">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="N50" t="s" s="0">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" s="0">
         <v>50</v>
       </c>
       <c r="C51" t="str" s="0">
         <f>Helper!D28</f>
-        <v>Silky Anteater</v>
+        <v>Mandarin Fish</v>
       </c>
       <c r="O51" t="str" s="0">
         <f>Helper!D61</f>
-        <v>Spotted sandpiper</v>
-      </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Swamp Nightjar</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" s="0">
         <v>51</v>
       </c>
       <c r="E52" t="s" s="0">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M52" t="s" s="0">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" s="0">
         <v>52</v>
       </c>
       <c r="C53" t="str" s="0">
         <f>Helper!D20</f>
-        <v>Dik Dik</v>
+        <v>Wolf's Mona Monkey</v>
       </c>
       <c r="O53" t="str" s="0">
         <f>Helper!D53</f>
-        <v>Wolverine</v>
-      </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Great White Shark</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" s="0">
         <v>53</v>
       </c>
       <c r="D54" t="s" s="0">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="N54" t="s" s="0">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" s="0">
         <v>54</v>
       </c>
       <c r="C55" t="str" s="0">
         <f>Helper!D31</f>
-        <v>Colo Colo Opossum</v>
+        <v>Flat Lizard</v>
       </c>
       <c r="O55" t="str" s="0">
         <f>Helper!D64</f>
-        <v>Giant Water Bug</v>
-      </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Elegant Dancing Frog</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" s="0">
         <v>55</v>
       </c>
       <c r="F56" t="s" s="0">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="L56" t="s" s="0">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="0">
         <v>56</v>
       </c>
       <c r="C57" t="str" s="0">
         <f>Helper!D24</f>
-        <v>Bulldog Bat</v>
+        <v xml:space="preserve">Golden-headed Lion Tamarin </v>
       </c>
       <c r="O57" t="str" s="0">
         <f>Helper!D57</f>
-        <v>Greater Flamingo</v>
-      </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Coral Snake</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" s="0">
         <v>57</v>
       </c>
       <c r="D58" t="s" s="0">
-        <v>38</v>
+        <v>87</v>
       </c>
       <c r="N58" t="s" s="0">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" s="0">
         <v>58</v>
       </c>
       <c r="C59" t="str" s="0">
         <f>Helper!D27</f>
-        <v>Thor's Hero Shrew</v>
+        <v>Mottled Cup Moth</v>
       </c>
       <c r="O59" t="str" s="0">
         <f>Helper!D60</f>
-        <v>Dyak Fruit Bat</v>
-      </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Flame Bowerbird</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" s="0">
         <v>59</v>
       </c>
       <c r="E60" t="s" s="0">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="M60" t="s" s="0">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" s="0">
         <v>60</v>
       </c>
       <c r="C61" t="str" s="0">
         <f>Helper!D19</f>
-        <v xml:space="preserve">Rock Hyrax </v>
+        <v>Red-shanked Douc</v>
       </c>
       <c r="O61" t="str" s="0">
         <f>Helper!D52</f>
-        <v>Greater Rhea</v>
-      </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
+        <v>Forest Elephant</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" s="0">
         <v>61</v>
       </c>
       <c r="D62" t="s" s="0">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="N62" t="s" s="0">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" s="0">
         <v>62</v>
       </c>
       <c r="C63" t="str" s="0">
         <f>Helper!D32</f>
-        <v>Pygmy Jerboa</v>
+        <v>Rainbow Scarab</v>
       </c>
       <c r="O63" t="str" s="0">
         <f>Helper!D65</f>
-        <v xml:space="preserve">Three-Spined stickleback </v>
+        <v>Honey Bee</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tried to fix sizing, almost done
</commit_message>
<xml_diff>
--- a/Resources/Bracket.xlsx
+++ b/Resources/Bracket.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2198" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3437" uniqueCount="114">
   <si>
     <t>Type in the two Wildcard animals below</t>
   </si>
@@ -364,6 +364,9 @@
   </si>
   <si>
     <t>Bornean Rainbow Toad</t>
+  </si>
+  <si>
+    <t>Schizomid</t>
   </si>
 </sst>
 </file>
@@ -2847,7 +2850,7 @@
         <v>7</v>
       </c>
       <c r="F8" t="s" s="0">
-        <v>96</v>
+        <v>53</v>
       </c>
       <c r="L8" t="s" s="0">
         <v>65</v>
@@ -2871,10 +2874,10 @@
         <v>9</v>
       </c>
       <c r="D10" t="s" s="0">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="N10" t="s" s="0">
-        <v>104</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -2895,10 +2898,10 @@
         <v>11</v>
       </c>
       <c r="E12" t="s" s="0">
-        <v>96</v>
+        <v>53</v>
       </c>
       <c r="M12" t="s" s="0">
-        <v>104</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -2919,10 +2922,10 @@
         <v>13</v>
       </c>
       <c r="D14" t="s" s="0">
-        <v>96</v>
+        <v>53</v>
       </c>
       <c r="N14" t="s" s="0">
-        <v>68</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -2943,7 +2946,7 @@
         <v>15</v>
       </c>
       <c r="G16" t="s" s="0">
-        <v>109</v>
+        <v>53</v>
       </c>
       <c r="K16" t="s" s="0">
         <v>65</v>
@@ -2967,10 +2970,10 @@
         <v>17</v>
       </c>
       <c r="D18" t="s" s="0">
-        <v>97</v>
+        <v>54</v>
       </c>
       <c r="N18" t="s" s="0">
-        <v>69</v>
+        <v>105</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
@@ -3039,7 +3042,7 @@
         <v>23</v>
       </c>
       <c r="F24" t="s" s="0">
-        <v>109</v>
+        <v>83</v>
       </c>
       <c r="L24" t="s" s="0">
         <v>106</v>
@@ -3063,10 +3066,10 @@
         <v>25</v>
       </c>
       <c r="D26" t="s" s="0">
-        <v>109</v>
+        <v>56</v>
       </c>
       <c r="N26" t="s" s="0">
-        <v>91</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
@@ -3087,7 +3090,7 @@
         <v>27</v>
       </c>
       <c r="E28" t="s" s="0">
-        <v>109</v>
+        <v>57</v>
       </c>
       <c r="M28" t="s" s="0">
         <v>106</v>
@@ -3111,7 +3114,7 @@
         <v>29</v>
       </c>
       <c r="D30" t="s" s="0">
-        <v>98</v>
+        <v>57</v>
       </c>
       <c r="N30" t="s" s="0">
         <v>106</v>
@@ -3135,13 +3138,13 @@
         <v>31</v>
       </c>
       <c r="H32" t="s" s="0">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="I32" t="s" s="0">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="J32" t="s" s="0">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
@@ -3166,7 +3169,7 @@
         <v>Sparklemuffin Peacock Spider</v>
       </c>
       <c r="D34" t="s" s="0">
-        <v>84</v>
+        <v>49</v>
       </c>
       <c r="N34" t="s" s="0">
         <v>73</v>
@@ -3177,7 +3180,7 @@
         <v>34</v>
       </c>
       <c r="C35" t="s" s="0">
-        <v>81</v>
+        <v>49</v>
       </c>
       <c r="O35" t="str" s="0">
         <f>Helper!D66</f>
@@ -3193,7 +3196,7 @@
         <v>Rainbow Grasshopper</v>
       </c>
       <c r="E36" t="s" s="0">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="M36" t="s" s="0">
         <v>73</v>
@@ -3217,7 +3220,7 @@
         <v>37</v>
       </c>
       <c r="D38" t="s" s="0">
-        <v>85</v>
+        <v>58</v>
       </c>
       <c r="N38" t="s" s="0">
         <v>101</v>
@@ -3241,7 +3244,7 @@
         <v>39</v>
       </c>
       <c r="F40" t="s" s="0">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="L40" t="s" s="0">
         <v>73</v>
@@ -3265,7 +3268,7 @@
         <v>41</v>
       </c>
       <c r="D42" t="s" s="0">
-        <v>112</v>
+        <v>59</v>
       </c>
       <c r="N42" t="s" s="0">
         <v>75</v>
@@ -3337,10 +3340,10 @@
         <v>47</v>
       </c>
       <c r="G48" t="s" s="0">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="K48" t="s" s="0">
-        <v>73</v>
+        <v>94</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
@@ -3361,7 +3364,7 @@
         <v>49</v>
       </c>
       <c r="D50" t="s" s="0">
-        <v>61</v>
+        <v>99</v>
       </c>
       <c r="N50" t="s" s="0">
         <v>107</v>
@@ -3385,10 +3388,10 @@
         <v>51</v>
       </c>
       <c r="E52" t="s" s="0">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="M52" t="s" s="0">
-        <v>107</v>
+        <v>94</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
@@ -3433,10 +3436,10 @@
         <v>55</v>
       </c>
       <c r="F56" t="s" s="0">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="L56" t="s" s="0">
-        <v>80</v>
+        <v>94</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
@@ -3484,7 +3487,7 @@
         <v>64</v>
       </c>
       <c r="M60" t="s" s="0">
-        <v>80</v>
+        <v>95</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Almost done with sizing, fic winner spacing.
</commit_message>
<xml_diff>
--- a/Resources/Bracket.xlsx
+++ b/Resources/Bracket.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3437" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5310" uniqueCount="114">
   <si>
     <t>Type in the two Wildcard animals below</t>
   </si>
@@ -2805,7 +2805,7 @@
         <v>50</v>
       </c>
       <c r="M4" t="s" s="0">
-        <v>65</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -2826,10 +2826,10 @@
         <v>5</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>108</v>
+        <v>51</v>
       </c>
       <c r="N6" t="s" s="0">
-        <v>66</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -2850,10 +2850,10 @@
         <v>7</v>
       </c>
       <c r="F8" t="s" s="0">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="L8" t="s" s="0">
-        <v>65</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -2874,10 +2874,10 @@
         <v>9</v>
       </c>
       <c r="D10" t="s" s="0">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="N10" t="s" s="0">
-        <v>67</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -2898,10 +2898,10 @@
         <v>11</v>
       </c>
       <c r="E12" t="s" s="0">
-        <v>53</v>
+        <v>82</v>
       </c>
       <c r="M12" t="s" s="0">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -2925,7 +2925,7 @@
         <v>53</v>
       </c>
       <c r="N14" t="s" s="0">
-        <v>89</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -2946,10 +2946,10 @@
         <v>15</v>
       </c>
       <c r="G16" t="s" s="0">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="K16" t="s" s="0">
-        <v>65</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -2970,10 +2970,10 @@
         <v>17</v>
       </c>
       <c r="D18" t="s" s="0">
-        <v>54</v>
+        <v>97</v>
       </c>
       <c r="N18" t="s" s="0">
-        <v>105</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
@@ -2994,10 +2994,10 @@
         <v>19</v>
       </c>
       <c r="E20" t="s" s="0">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c r="M20" t="s" s="0">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -3021,7 +3021,7 @@
         <v>83</v>
       </c>
       <c r="N22" t="s" s="0">
-        <v>70</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -3042,7 +3042,7 @@
         <v>23</v>
       </c>
       <c r="F24" t="s" s="0">
-        <v>83</v>
+        <v>109</v>
       </c>
       <c r="L24" t="s" s="0">
         <v>106</v>
@@ -3066,7 +3066,7 @@
         <v>25</v>
       </c>
       <c r="D26" t="s" s="0">
-        <v>56</v>
+        <v>109</v>
       </c>
       <c r="N26" t="s" s="0">
         <v>71</v>
@@ -3090,7 +3090,7 @@
         <v>27</v>
       </c>
       <c r="E28" t="s" s="0">
-        <v>57</v>
+        <v>109</v>
       </c>
       <c r="M28" t="s" s="0">
         <v>106</v>
@@ -3114,7 +3114,7 @@
         <v>29</v>
       </c>
       <c r="D30" t="s" s="0">
-        <v>57</v>
+        <v>98</v>
       </c>
       <c r="N30" t="s" s="0">
         <v>106</v>
@@ -3138,13 +3138,13 @@
         <v>31</v>
       </c>
       <c r="H32" t="s" s="0">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="I32" t="s" s="0">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="J32" t="s" s="0">
-        <v>65</v>
+        <v>106</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
@@ -3169,7 +3169,7 @@
         <v>Sparklemuffin Peacock Spider</v>
       </c>
       <c r="D34" t="s" s="0">
-        <v>49</v>
+        <v>84</v>
       </c>
       <c r="N34" t="s" s="0">
         <v>73</v>
@@ -3196,7 +3196,7 @@
         <v>Rainbow Grasshopper</v>
       </c>
       <c r="E36" t="s" s="0">
-        <v>58</v>
+        <v>84</v>
       </c>
       <c r="M36" t="s" s="0">
         <v>73</v>
@@ -3220,7 +3220,7 @@
         <v>37</v>
       </c>
       <c r="D38" t="s" s="0">
-        <v>58</v>
+        <v>85</v>
       </c>
       <c r="N38" t="s" s="0">
         <v>101</v>
@@ -3244,7 +3244,7 @@
         <v>39</v>
       </c>
       <c r="F40" t="s" s="0">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L40" t="s" s="0">
         <v>73</v>
@@ -3271,7 +3271,7 @@
         <v>59</v>
       </c>
       <c r="N42" t="s" s="0">
-        <v>75</v>
+        <v>92</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
@@ -3295,7 +3295,7 @@
         <v>60</v>
       </c>
       <c r="M44" t="s" s="0">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
@@ -3340,10 +3340,10 @@
         <v>47</v>
       </c>
       <c r="G48" t="s" s="0">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="K48" t="s" s="0">
-        <v>94</v>
+        <v>73</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
@@ -3364,10 +3364,10 @@
         <v>49</v>
       </c>
       <c r="D50" t="s" s="0">
-        <v>99</v>
+        <v>61</v>
       </c>
       <c r="N50" t="s" s="0">
-        <v>107</v>
+        <v>77</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
@@ -3391,7 +3391,7 @@
         <v>62</v>
       </c>
       <c r="M52" t="s" s="0">
-        <v>94</v>
+        <v>77</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
@@ -3415,7 +3415,7 @@
         <v>62</v>
       </c>
       <c r="N54" t="s" s="0">
-        <v>94</v>
+        <v>78</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
@@ -3439,7 +3439,7 @@
         <v>64</v>
       </c>
       <c r="L56" t="s" s="0">
-        <v>94</v>
+        <v>77</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
@@ -3463,7 +3463,7 @@
         <v>87</v>
       </c>
       <c r="N58" t="s" s="0">
-        <v>95</v>
+        <v>79</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
@@ -3487,7 +3487,7 @@
         <v>64</v>
       </c>
       <c r="M60" t="s" s="0">
-        <v>95</v>
+        <v>111</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
@@ -3511,7 +3511,7 @@
         <v>64</v>
       </c>
       <c r="N62" t="s" s="0">
-        <v>80</v>
+        <v>111</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finally done with spacing, could work more to make it look good enough, but it's fine for now.
</commit_message>
<xml_diff>
--- a/Resources/Bracket.xlsx
+++ b/Resources/Bracket.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5310" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5725" uniqueCount="114">
   <si>
     <t>Type in the two Wildcard animals below</t>
   </si>
@@ -2802,10 +2802,10 @@
         <v>3</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>50</v>
+        <v>108</v>
       </c>
       <c r="M4" t="s" s="0">
-        <v>88</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -2826,7 +2826,7 @@
         <v>5</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>51</v>
+        <v>108</v>
       </c>
       <c r="N6" t="s" s="0">
         <v>88</v>
@@ -2850,10 +2850,10 @@
         <v>7</v>
       </c>
       <c r="F8" t="s" s="0">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L8" t="s" s="0">
-        <v>88</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -2874,7 +2874,7 @@
         <v>9</v>
       </c>
       <c r="D10" t="s" s="0">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="N10" t="s" s="0">
         <v>104</v>
@@ -2898,7 +2898,7 @@
         <v>11</v>
       </c>
       <c r="E12" t="s" s="0">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="M12" t="s" s="0">
         <v>68</v>
@@ -2925,7 +2925,7 @@
         <v>53</v>
       </c>
       <c r="N14" t="s" s="0">
-        <v>68</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -2946,10 +2946,10 @@
         <v>15</v>
       </c>
       <c r="G16" t="s" s="0">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="K16" t="s" s="0">
-        <v>106</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -2973,7 +2973,7 @@
         <v>97</v>
       </c>
       <c r="N18" t="s" s="0">
-        <v>69</v>
+        <v>105</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
@@ -2994,7 +2994,7 @@
         <v>19</v>
       </c>
       <c r="E20" t="s" s="0">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="M20" t="s" s="0">
         <v>69</v>
@@ -3021,7 +3021,7 @@
         <v>83</v>
       </c>
       <c r="N22" t="s" s="0">
-        <v>90</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -3042,10 +3042,10 @@
         <v>23</v>
       </c>
       <c r="F24" t="s" s="0">
-        <v>109</v>
+        <v>57</v>
       </c>
       <c r="L24" t="s" s="0">
-        <v>106</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
@@ -3090,10 +3090,10 @@
         <v>27</v>
       </c>
       <c r="E28" t="s" s="0">
-        <v>109</v>
+        <v>57</v>
       </c>
       <c r="M28" t="s" s="0">
-        <v>106</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
@@ -3117,7 +3117,7 @@
         <v>98</v>
       </c>
       <c r="N30" t="s" s="0">
-        <v>106</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
@@ -3138,13 +3138,13 @@
         <v>31</v>
       </c>
       <c r="H32" t="s" s="0">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="I32" t="s" s="0">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="J32" t="s" s="0">
-        <v>106</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
@@ -3180,7 +3180,7 @@
         <v>34</v>
       </c>
       <c r="C35" t="s" s="0">
-        <v>49</v>
+        <v>81</v>
       </c>
       <c r="O35" t="str" s="0">
         <f>Helper!D66</f>
@@ -3244,7 +3244,7 @@
         <v>39</v>
       </c>
       <c r="F40" t="s" s="0">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="L40" t="s" s="0">
         <v>73</v>
@@ -3271,7 +3271,7 @@
         <v>59</v>
       </c>
       <c r="N42" t="s" s="0">
-        <v>92</v>
+        <v>75</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
@@ -3292,10 +3292,10 @@
         <v>43</v>
       </c>
       <c r="E44" t="s" s="0">
-        <v>60</v>
+        <v>86</v>
       </c>
       <c r="M44" t="s" s="0">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
@@ -3340,7 +3340,7 @@
         <v>47</v>
       </c>
       <c r="G48" t="s" s="0">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="K48" t="s" s="0">
         <v>73</v>
@@ -3388,10 +3388,10 @@
         <v>51</v>
       </c>
       <c r="E52" t="s" s="0">
-        <v>62</v>
+        <v>110</v>
       </c>
       <c r="M52" t="s" s="0">
-        <v>77</v>
+        <v>94</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
@@ -3412,10 +3412,10 @@
         <v>53</v>
       </c>
       <c r="D54" t="s" s="0">
-        <v>62</v>
+        <v>110</v>
       </c>
       <c r="N54" t="s" s="0">
-        <v>78</v>
+        <v>94</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
@@ -3439,7 +3439,7 @@
         <v>64</v>
       </c>
       <c r="L56" t="s" s="0">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
@@ -3460,7 +3460,7 @@
         <v>57</v>
       </c>
       <c r="D58" t="s" s="0">
-        <v>87</v>
+        <v>63</v>
       </c>
       <c r="N58" t="s" s="0">
         <v>79</v>
@@ -3487,7 +3487,7 @@
         <v>64</v>
       </c>
       <c r="M60" t="s" s="0">
-        <v>111</v>
+        <v>80</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
@@ -3511,7 +3511,7 @@
         <v>64</v>
       </c>
       <c r="N62" t="s" s="0">
-        <v>111</v>
+        <v>80</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Need to fix window closing when trying to autofill will always close the window even if the user selected no
</commit_message>
<xml_diff>
--- a/Resources/Bracket.xlsx
+++ b/Resources/Bracket.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5725" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5909" uniqueCount="114">
   <si>
     <t>Type in the two Wildcard animals below</t>
   </si>
@@ -2802,7 +2802,7 @@
         <v>3</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>108</v>
+        <v>50</v>
       </c>
       <c r="M4" t="s" s="0">
         <v>65</v>
@@ -2826,10 +2826,10 @@
         <v>5</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>108</v>
+        <v>51</v>
       </c>
       <c r="N6" t="s" s="0">
-        <v>88</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -2853,7 +2853,7 @@
         <v>52</v>
       </c>
       <c r="L8" t="s" s="0">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -2874,7 +2874,7 @@
         <v>9</v>
       </c>
       <c r="D10" t="s" s="0">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="N10" t="s" s="0">
         <v>104</v>
@@ -2898,10 +2898,10 @@
         <v>11</v>
       </c>
       <c r="E12" t="s" s="0">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="M12" t="s" s="0">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -2925,7 +2925,7 @@
         <v>53</v>
       </c>
       <c r="N14" t="s" s="0">
-        <v>89</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -2946,10 +2946,10 @@
         <v>15</v>
       </c>
       <c r="G16" t="s" s="0">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="K16" t="s" s="0">
-        <v>65</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -2970,10 +2970,10 @@
         <v>17</v>
       </c>
       <c r="D18" t="s" s="0">
-        <v>97</v>
+        <v>54</v>
       </c>
       <c r="N18" t="s" s="0">
-        <v>105</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
@@ -2994,7 +2994,7 @@
         <v>19</v>
       </c>
       <c r="E20" t="s" s="0">
-        <v>83</v>
+        <v>54</v>
       </c>
       <c r="M20" t="s" s="0">
         <v>69</v>
@@ -3018,10 +3018,10 @@
         <v>21</v>
       </c>
       <c r="D22" t="s" s="0">
-        <v>83</v>
+        <v>55</v>
       </c>
       <c r="N22" t="s" s="0">
-        <v>70</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -3042,10 +3042,10 @@
         <v>23</v>
       </c>
       <c r="F24" t="s" s="0">
-        <v>57</v>
+        <v>83</v>
       </c>
       <c r="L24" t="s" s="0">
-        <v>69</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
@@ -3093,7 +3093,7 @@
         <v>57</v>
       </c>
       <c r="M28" t="s" s="0">
-        <v>91</v>
+        <v>106</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
@@ -3114,10 +3114,10 @@
         <v>29</v>
       </c>
       <c r="D30" t="s" s="0">
-        <v>98</v>
+        <v>57</v>
       </c>
       <c r="N30" t="s" s="0">
-        <v>72</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
@@ -3138,13 +3138,13 @@
         <v>31</v>
       </c>
       <c r="H32" t="s" s="0">
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="I32" t="s" s="0">
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="J32" t="s" s="0">
-        <v>73</v>
+        <v>106</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
@@ -3180,7 +3180,7 @@
         <v>34</v>
       </c>
       <c r="C35" t="s" s="0">
-        <v>81</v>
+        <v>49</v>
       </c>
       <c r="O35" t="str" s="0">
         <f>Helper!D66</f>
@@ -3220,10 +3220,10 @@
         <v>37</v>
       </c>
       <c r="D38" t="s" s="0">
-        <v>85</v>
+        <v>58</v>
       </c>
       <c r="N38" t="s" s="0">
-        <v>101</v>
+        <v>74</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
@@ -3247,7 +3247,7 @@
         <v>84</v>
       </c>
       <c r="L40" t="s" s="0">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
@@ -3268,10 +3268,10 @@
         <v>41</v>
       </c>
       <c r="D42" t="s" s="0">
-        <v>59</v>
+        <v>112</v>
       </c>
       <c r="N42" t="s" s="0">
-        <v>75</v>
+        <v>92</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
@@ -3292,10 +3292,10 @@
         <v>43</v>
       </c>
       <c r="E44" t="s" s="0">
-        <v>86</v>
+        <v>60</v>
       </c>
       <c r="M44" t="s" s="0">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
@@ -3319,7 +3319,7 @@
         <v>60</v>
       </c>
       <c r="N46" t="s" s="0">
-        <v>93</v>
+        <v>76</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
@@ -3343,7 +3343,7 @@
         <v>84</v>
       </c>
       <c r="K48" t="s" s="0">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
@@ -3388,10 +3388,10 @@
         <v>51</v>
       </c>
       <c r="E52" t="s" s="0">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="M52" t="s" s="0">
-        <v>94</v>
+        <v>77</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
@@ -3415,7 +3415,7 @@
         <v>110</v>
       </c>
       <c r="N54" t="s" s="0">
-        <v>94</v>
+        <v>78</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
@@ -3463,7 +3463,7 @@
         <v>63</v>
       </c>
       <c r="N58" t="s" s="0">
-        <v>79</v>
+        <v>95</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>